<commit_message>
fixed gannt chart dates
</commit_message>
<xml_diff>
--- a/docs/planningdocuments/gannt/GanttChart_POS_9.xlsx
+++ b/docs/planningdocuments/gannt/GanttChart_POS_9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CPS353-POS\docs\planningdocuments\gannt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80A6F0C5-1585-4926-AE52-E031CB0CABFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB277CE-D411-462B-B8AA-F68179E6CC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>W5 10/6/2022</t>
-  </si>
-  <si>
-    <t>W9 11/3/2022</t>
   </si>
   <si>
     <t>Financial</t>
@@ -463,9 +460,6 @@
     <t xml:space="preserve">Create password hashing function </t>
   </si>
   <si>
-    <t>Change DB Connector to PDO</t>
-  </si>
-  <si>
     <t>Integrate Security and User Classes</t>
   </si>
   <si>
@@ -523,25 +517,28 @@
     <t>W8 10/24/2022</t>
   </si>
   <si>
-    <t>W10 10/31/2022</t>
-  </si>
-  <si>
-    <t>W11 11/7/2022</t>
-  </si>
-  <si>
-    <t>W12 11/14/2022</t>
-  </si>
-  <si>
-    <t>W13 11/21/2022</t>
-  </si>
-  <si>
-    <t>W14 11/28/2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">Add Data Validation to Admin Invetory </t>
   </si>
   <si>
     <t>Get Admin Page Connected to DB</t>
+  </si>
+  <si>
+    <t>W9 10/31/2022</t>
+  </si>
+  <si>
+    <t>W10  11/7/22</t>
+  </si>
+  <si>
+    <t>W11 11/14/2022</t>
+  </si>
+  <si>
+    <t>W12 11/21/2022</t>
+  </si>
+  <si>
+    <t>W13 11/28/2022</t>
+  </si>
+  <si>
+    <t>W14 12/5/2022</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1545,27 +1542,6 @@
     <xf numFmtId="0" fontId="27" fillId="28" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1580,9 +1556,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1591,6 +1572,25 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1911,10 +1911,10 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BZ115"/>
+  <dimension ref="A1:BZ116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2012,38 +2012,38 @@
     </row>
     <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="167"/>
-      <c r="P2" s="165"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="165"/>
-      <c r="S2" s="165"/>
-      <c r="T2" s="165"/>
-      <c r="U2" s="165"/>
-      <c r="V2" s="165"/>
-      <c r="W2" s="165"/>
-      <c r="X2" s="165"/>
-      <c r="Y2" s="165"/>
-      <c r="Z2" s="165"/>
-      <c r="AA2" s="165"/>
-      <c r="AB2" s="165"/>
-      <c r="AC2" s="165"/>
-      <c r="AD2" s="165"/>
-      <c r="AE2" s="165"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="156"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
+      <c r="T2" s="154"/>
+      <c r="U2" s="154"/>
+      <c r="V2" s="154"/>
+      <c r="W2" s="154"/>
+      <c r="X2" s="154"/>
+      <c r="Y2" s="154"/>
+      <c r="Z2" s="154"/>
+      <c r="AA2" s="154"/>
+      <c r="AB2" s="154"/>
+      <c r="AC2" s="154"/>
+      <c r="AD2" s="154"/>
+      <c r="AE2" s="154"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -2178,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="158"/>
-      <c r="D4" s="168" t="s">
+      <c r="D4" s="159" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="160"/>
@@ -2194,7 +2194,7 @@
       <c r="M4" s="158"/>
       <c r="N4" s="158"/>
       <c r="O4" s="158"/>
-      <c r="P4" s="169" t="s">
+      <c r="P4" s="161" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="160"/>
@@ -2266,7 +2266,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="158"/>
-      <c r="D5" s="159" t="s">
+      <c r="D5" s="171" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="160"/>
@@ -2282,7 +2282,7 @@
       <c r="M5" s="158"/>
       <c r="N5" s="158"/>
       <c r="O5" s="158"/>
-      <c r="P5" s="161">
+      <c r="P5" s="172">
         <v>44858</v>
       </c>
       <c r="Q5" s="160"/>
@@ -2598,205 +2598,205 @@
     </row>
     <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="162" t="s">
+      <c r="C9" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="162" t="s">
+      <c r="D9" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="162" t="s">
+      <c r="E9" s="151" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="162" t="s">
+      <c r="F9" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="162" t="s">
+      <c r="G9" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="170" t="s">
+      <c r="H9" s="162" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="172"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="152"/>
-      <c r="L9" s="152"/>
-      <c r="M9" s="152"/>
-      <c r="N9" s="152"/>
-      <c r="O9" s="152"/>
-      <c r="P9" s="152"/>
-      <c r="Q9" s="152"/>
-      <c r="R9" s="152"/>
-      <c r="S9" s="152"/>
-      <c r="T9" s="152"/>
-      <c r="U9" s="152"/>
-      <c r="V9" s="152"/>
-      <c r="W9" s="152"/>
-      <c r="X9" s="151"/>
-      <c r="Y9" s="152"/>
-      <c r="Z9" s="152"/>
-      <c r="AA9" s="152"/>
-      <c r="AB9" s="152"/>
-      <c r="AC9" s="152"/>
-      <c r="AD9" s="152"/>
-      <c r="AE9" s="152"/>
-      <c r="AF9" s="152"/>
-      <c r="AG9" s="152"/>
-      <c r="AH9" s="152"/>
-      <c r="AI9" s="152"/>
-      <c r="AJ9" s="152"/>
-      <c r="AK9" s="152"/>
-      <c r="AL9" s="152"/>
-      <c r="AM9" s="151"/>
-      <c r="AN9" s="152"/>
-      <c r="AO9" s="152"/>
-      <c r="AP9" s="152"/>
-      <c r="AQ9" s="152"/>
-      <c r="AR9" s="152"/>
-      <c r="AS9" s="152"/>
-      <c r="AT9" s="152"/>
-      <c r="AU9" s="152"/>
-      <c r="AV9" s="152"/>
-      <c r="AW9" s="152"/>
-      <c r="AX9" s="152"/>
-      <c r="AY9" s="152"/>
-      <c r="AZ9" s="152"/>
-      <c r="BA9" s="152"/>
-      <c r="BB9" s="151"/>
-      <c r="BC9" s="152"/>
-      <c r="BD9" s="152"/>
-      <c r="BE9" s="152"/>
-      <c r="BF9" s="152"/>
-      <c r="BG9" s="152"/>
-      <c r="BH9" s="152"/>
-      <c r="BI9" s="152"/>
-      <c r="BJ9" s="152"/>
-      <c r="BK9" s="152"/>
-      <c r="BL9" s="152"/>
-      <c r="BM9" s="152"/>
-      <c r="BN9" s="152"/>
-      <c r="BO9" s="152"/>
-      <c r="BP9" s="152"/>
-      <c r="BQ9" s="152"/>
-      <c r="BR9" s="152"/>
-      <c r="BS9" s="152"/>
-      <c r="BT9" s="152"/>
-      <c r="BU9" s="152"/>
-      <c r="BV9" s="152"/>
-      <c r="BW9" s="152"/>
-      <c r="BX9" s="152"/>
-      <c r="BY9" s="152"/>
-      <c r="BZ9" s="153"/>
+      <c r="I9" s="164"/>
+      <c r="J9" s="165"/>
+      <c r="K9" s="165"/>
+      <c r="L9" s="165"/>
+      <c r="M9" s="165"/>
+      <c r="N9" s="165"/>
+      <c r="O9" s="165"/>
+      <c r="P9" s="165"/>
+      <c r="Q9" s="165"/>
+      <c r="R9" s="165"/>
+      <c r="S9" s="165"/>
+      <c r="T9" s="165"/>
+      <c r="U9" s="165"/>
+      <c r="V9" s="165"/>
+      <c r="W9" s="165"/>
+      <c r="X9" s="166"/>
+      <c r="Y9" s="165"/>
+      <c r="Z9" s="165"/>
+      <c r="AA9" s="165"/>
+      <c r="AB9" s="165"/>
+      <c r="AC9" s="165"/>
+      <c r="AD9" s="165"/>
+      <c r="AE9" s="165"/>
+      <c r="AF9" s="165"/>
+      <c r="AG9" s="165"/>
+      <c r="AH9" s="165"/>
+      <c r="AI9" s="165"/>
+      <c r="AJ9" s="165"/>
+      <c r="AK9" s="165"/>
+      <c r="AL9" s="165"/>
+      <c r="AM9" s="166"/>
+      <c r="AN9" s="165"/>
+      <c r="AO9" s="165"/>
+      <c r="AP9" s="165"/>
+      <c r="AQ9" s="165"/>
+      <c r="AR9" s="165"/>
+      <c r="AS9" s="165"/>
+      <c r="AT9" s="165"/>
+      <c r="AU9" s="165"/>
+      <c r="AV9" s="165"/>
+      <c r="AW9" s="165"/>
+      <c r="AX9" s="165"/>
+      <c r="AY9" s="165"/>
+      <c r="AZ9" s="165"/>
+      <c r="BA9" s="165"/>
+      <c r="BB9" s="166"/>
+      <c r="BC9" s="165"/>
+      <c r="BD9" s="165"/>
+      <c r="BE9" s="165"/>
+      <c r="BF9" s="165"/>
+      <c r="BG9" s="165"/>
+      <c r="BH9" s="165"/>
+      <c r="BI9" s="165"/>
+      <c r="BJ9" s="165"/>
+      <c r="BK9" s="165"/>
+      <c r="BL9" s="165"/>
+      <c r="BM9" s="165"/>
+      <c r="BN9" s="165"/>
+      <c r="BO9" s="165"/>
+      <c r="BP9" s="165"/>
+      <c r="BQ9" s="165"/>
+      <c r="BR9" s="165"/>
+      <c r="BS9" s="165"/>
+      <c r="BT9" s="165"/>
+      <c r="BU9" s="165"/>
+      <c r="BV9" s="165"/>
+      <c r="BW9" s="165"/>
+      <c r="BX9" s="165"/>
+      <c r="BY9" s="165"/>
+      <c r="BZ9" s="170"/>
     </row>
     <row r="10" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
-      <c r="B10" s="163"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="163"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="163"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="154" t="s">
+      <c r="B10" s="152"/>
+      <c r="C10" s="152"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="152"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="167" t="s">
         <v>95</v>
       </c>
-      <c r="J10" s="155"/>
-      <c r="K10" s="155"/>
-      <c r="L10" s="155"/>
-      <c r="M10" s="156"/>
-      <c r="N10" s="154" t="s">
+      <c r="J10" s="168"/>
+      <c r="K10" s="168"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="169"/>
+      <c r="N10" s="167" t="s">
         <v>96</v>
       </c>
-      <c r="O10" s="155"/>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="155"/>
-      <c r="R10" s="156"/>
-      <c r="S10" s="154" t="s">
+      <c r="O10" s="168"/>
+      <c r="P10" s="168"/>
+      <c r="Q10" s="168"/>
+      <c r="R10" s="169"/>
+      <c r="S10" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="T10" s="155"/>
-      <c r="U10" s="155"/>
-      <c r="V10" s="155"/>
-      <c r="W10" s="156"/>
-      <c r="X10" s="154" t="s">
+      <c r="T10" s="168"/>
+      <c r="U10" s="168"/>
+      <c r="V10" s="168"/>
+      <c r="W10" s="169"/>
+      <c r="X10" s="167" t="s">
         <v>103</v>
       </c>
-      <c r="Y10" s="155"/>
-      <c r="Z10" s="155"/>
-      <c r="AA10" s="155"/>
-      <c r="AB10" s="156"/>
-      <c r="AC10" s="154" t="s">
+      <c r="Y10" s="168"/>
+      <c r="Z10" s="168"/>
+      <c r="AA10" s="168"/>
+      <c r="AB10" s="169"/>
+      <c r="AC10" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="AD10" s="155"/>
-      <c r="AE10" s="155"/>
-      <c r="AF10" s="155"/>
-      <c r="AG10" s="156"/>
-      <c r="AH10" s="154" t="s">
+      <c r="AD10" s="168"/>
+      <c r="AE10" s="168"/>
+      <c r="AF10" s="168"/>
+      <c r="AG10" s="169"/>
+      <c r="AH10" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="AI10" s="155"/>
-      <c r="AJ10" s="155"/>
-      <c r="AK10" s="155"/>
-      <c r="AL10" s="156"/>
-      <c r="AM10" s="154" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN10" s="155"/>
-      <c r="AO10" s="155"/>
-      <c r="AP10" s="155"/>
-      <c r="AQ10" s="156"/>
-      <c r="AR10" s="154" t="s">
-        <v>134</v>
-      </c>
-      <c r="AS10" s="155"/>
-      <c r="AT10" s="155"/>
-      <c r="AU10" s="155"/>
-      <c r="AV10" s="156"/>
-      <c r="AW10" s="154" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX10" s="155"/>
-      <c r="AY10" s="155"/>
-      <c r="AZ10" s="155"/>
-      <c r="BA10" s="156"/>
-      <c r="BB10" s="154" t="s">
+      <c r="AI10" s="168"/>
+      <c r="AJ10" s="168"/>
+      <c r="AK10" s="168"/>
+      <c r="AL10" s="169"/>
+      <c r="AM10" s="167" t="s">
+        <v>131</v>
+      </c>
+      <c r="AN10" s="168"/>
+      <c r="AO10" s="168"/>
+      <c r="AP10" s="168"/>
+      <c r="AQ10" s="169"/>
+      <c r="AR10" s="167" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS10" s="168"/>
+      <c r="AT10" s="168"/>
+      <c r="AU10" s="168"/>
+      <c r="AV10" s="169"/>
+      <c r="AW10" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="BC10" s="155"/>
-      <c r="BD10" s="155"/>
-      <c r="BE10" s="155"/>
-      <c r="BF10" s="156"/>
-      <c r="BG10" s="154" t="s">
+      <c r="AX10" s="168"/>
+      <c r="AY10" s="168"/>
+      <c r="AZ10" s="168"/>
+      <c r="BA10" s="169"/>
+      <c r="BB10" s="167" t="s">
         <v>136</v>
       </c>
-      <c r="BH10" s="155"/>
-      <c r="BI10" s="155"/>
-      <c r="BJ10" s="155"/>
-      <c r="BK10" s="156"/>
-      <c r="BL10" s="154" t="s">
+      <c r="BC10" s="168"/>
+      <c r="BD10" s="168"/>
+      <c r="BE10" s="168"/>
+      <c r="BF10" s="169"/>
+      <c r="BG10" s="167" t="s">
         <v>137</v>
       </c>
-      <c r="BM10" s="155"/>
-      <c r="BN10" s="155"/>
-      <c r="BO10" s="155"/>
-      <c r="BP10" s="156"/>
-      <c r="BQ10" s="154" t="s">
+      <c r="BH10" s="168"/>
+      <c r="BI10" s="168"/>
+      <c r="BJ10" s="168"/>
+      <c r="BK10" s="169"/>
+      <c r="BL10" s="167" t="s">
         <v>138</v>
       </c>
-      <c r="BR10" s="155"/>
-      <c r="BS10" s="155"/>
-      <c r="BT10" s="155"/>
-      <c r="BU10" s="156"/>
-      <c r="BV10" s="154" t="s">
+      <c r="BM10" s="168"/>
+      <c r="BN10" s="168"/>
+      <c r="BO10" s="168"/>
+      <c r="BP10" s="169"/>
+      <c r="BQ10" s="167" t="s">
         <v>139</v>
       </c>
-      <c r="BW10" s="155"/>
-      <c r="BX10" s="155"/>
-      <c r="BY10" s="155"/>
-      <c r="BZ10" s="156"/>
+      <c r="BR10" s="168"/>
+      <c r="BS10" s="168"/>
+      <c r="BT10" s="168"/>
+      <c r="BU10" s="169"/>
+      <c r="BV10" s="167" t="s">
+        <v>140</v>
+      </c>
+      <c r="BW10" s="168"/>
+      <c r="BX10" s="168"/>
+      <c r="BY10" s="168"/>
+      <c r="BZ10" s="169"/>
     </row>
     <row r="11" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
@@ -5274,7 +5274,7 @@
       <c r="A37" s="134"/>
       <c r="B37" s="135"/>
       <c r="C37" s="136" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D37" s="137"/>
       <c r="E37" s="137"/>
@@ -5438,7 +5438,7 @@
       <c r="A39" s="21"/>
       <c r="B39" s="85"/>
       <c r="C39" s="120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="87"/>
       <c r="E39" s="87"/>
@@ -5519,7 +5519,7 @@
       <c r="A40" s="21"/>
       <c r="B40" s="85"/>
       <c r="C40" s="120" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D40" s="87"/>
       <c r="E40" s="87"/>
@@ -5601,7 +5601,7 @@
       <c r="A41" s="21"/>
       <c r="B41" s="85"/>
       <c r="C41" s="120" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D41" s="87"/>
       <c r="E41" s="87"/>
@@ -5683,7 +5683,7 @@
       <c r="A42" s="21"/>
       <c r="B42" s="85"/>
       <c r="C42" s="120" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D42" s="87"/>
       <c r="E42" s="87"/>
@@ -6089,7 +6089,7 @@
       <c r="A47" s="21"/>
       <c r="B47" s="85"/>
       <c r="C47" s="120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D47" s="87"/>
       <c r="E47" s="87"/>
@@ -6171,7 +6171,7 @@
       <c r="A48" s="21"/>
       <c r="B48" s="85"/>
       <c r="C48" s="120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D48" s="87"/>
       <c r="E48" s="87"/>
@@ -6210,25 +6210,25 @@
       <c r="AL48" s="88"/>
       <c r="AM48" s="88"/>
       <c r="AN48" s="88"/>
-      <c r="AO48" s="121"/>
-      <c r="AP48" s="121"/>
-      <c r="AQ48" s="121"/>
-      <c r="AR48" s="122"/>
-      <c r="AS48" s="88"/>
-      <c r="AT48" s="88"/>
-      <c r="AU48" s="88"/>
-      <c r="AV48" s="88"/>
-      <c r="AW48" s="88"/>
-      <c r="AX48" s="88"/>
-      <c r="AY48" s="88"/>
-      <c r="AZ48" s="88"/>
-      <c r="BA48" s="88"/>
-      <c r="BB48" s="88"/>
-      <c r="BC48" s="88"/>
-      <c r="BD48" s="88"/>
-      <c r="BE48" s="88"/>
-      <c r="BF48" s="88"/>
-      <c r="BG48" s="88"/>
+      <c r="AO48" s="173"/>
+      <c r="AP48" s="173"/>
+      <c r="AQ48" s="173"/>
+      <c r="AR48" s="173"/>
+      <c r="AS48" s="173"/>
+      <c r="AT48" s="173"/>
+      <c r="AU48" s="173"/>
+      <c r="AV48" s="173"/>
+      <c r="AW48" s="121"/>
+      <c r="AX48" s="121"/>
+      <c r="AY48" s="121"/>
+      <c r="AZ48" s="121"/>
+      <c r="BA48" s="121"/>
+      <c r="BB48" s="121"/>
+      <c r="BC48" s="121"/>
+      <c r="BD48" s="121"/>
+      <c r="BE48" s="121"/>
+      <c r="BF48" s="121"/>
+      <c r="BG48" s="122"/>
       <c r="BH48" s="88"/>
       <c r="BI48" s="88"/>
       <c r="BJ48" s="88"/>
@@ -6252,9 +6252,7 @@
     <row r="49" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="85"/>
-      <c r="C49" s="120" t="s">
-        <v>116</v>
-      </c>
+      <c r="C49" s="120"/>
       <c r="D49" s="87"/>
       <c r="E49" s="87"/>
       <c r="F49" s="87"/>
@@ -6292,14 +6290,14 @@
       <c r="AL49" s="88"/>
       <c r="AM49" s="88"/>
       <c r="AN49" s="88"/>
-      <c r="AO49" s="121"/>
-      <c r="AP49" s="121"/>
-      <c r="AQ49" s="121"/>
-      <c r="AR49" s="121"/>
-      <c r="AS49" s="121"/>
-      <c r="AT49" s="122"/>
-      <c r="AU49" s="122"/>
-      <c r="AV49" s="122"/>
+      <c r="AO49" s="173"/>
+      <c r="AP49" s="173"/>
+      <c r="AQ49" s="173"/>
+      <c r="AR49" s="173"/>
+      <c r="AS49" s="173"/>
+      <c r="AT49" s="173"/>
+      <c r="AU49" s="173"/>
+      <c r="AV49" s="173"/>
       <c r="AW49" s="88"/>
       <c r="AX49" s="88"/>
       <c r="AY49" s="88"/>
@@ -6334,7 +6332,7 @@
     <row r="50" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="85"/>
-      <c r="C50" s="86"/>
+      <c r="C50" s="120"/>
       <c r="D50" s="87"/>
       <c r="E50" s="87"/>
       <c r="F50" s="87"/>
@@ -6372,14 +6370,14 @@
       <c r="AL50" s="88"/>
       <c r="AM50" s="88"/>
       <c r="AN50" s="88"/>
-      <c r="AO50" s="88"/>
-      <c r="AP50" s="88"/>
-      <c r="AQ50" s="88"/>
-      <c r="AR50" s="88"/>
-      <c r="AS50" s="88"/>
-      <c r="AT50" s="88"/>
-      <c r="AU50" s="88"/>
-      <c r="AV50" s="88"/>
+      <c r="AO50" s="173"/>
+      <c r="AP50" s="173"/>
+      <c r="AQ50" s="173"/>
+      <c r="AR50" s="173"/>
+      <c r="AS50" s="173"/>
+      <c r="AT50" s="173"/>
+      <c r="AU50" s="173"/>
+      <c r="AV50" s="173"/>
       <c r="AW50" s="88"/>
       <c r="AX50" s="88"/>
       <c r="AY50" s="88"/>
@@ -6491,169 +6489,167 @@
       <c r="BY51" s="88"/>
       <c r="BZ51" s="88"/>
     </row>
-    <row r="52" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="72"/>
-      <c r="B52" s="73"/>
-      <c r="C52" s="76" t="s">
+    <row r="52" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="87"/>
+      <c r="E52" s="87"/>
+      <c r="F52" s="87"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="87"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="89"/>
+      <c r="K52" s="90"/>
+      <c r="L52" s="90"/>
+      <c r="M52" s="88"/>
+      <c r="N52" s="88"/>
+      <c r="O52" s="88"/>
+      <c r="P52" s="88"/>
+      <c r="Q52" s="88"/>
+      <c r="R52" s="88"/>
+      <c r="S52" s="88"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="88"/>
+      <c r="V52" s="88"/>
+      <c r="W52" s="88"/>
+      <c r="X52" s="88"/>
+      <c r="Y52" s="88"/>
+      <c r="Z52" s="88"/>
+      <c r="AA52" s="88"/>
+      <c r="AB52" s="88"/>
+      <c r="AC52" s="88"/>
+      <c r="AD52" s="88"/>
+      <c r="AE52" s="88"/>
+      <c r="AF52" s="88"/>
+      <c r="AG52" s="88"/>
+      <c r="AH52" s="88"/>
+      <c r="AI52" s="88"/>
+      <c r="AJ52" s="88"/>
+      <c r="AK52" s="88"/>
+      <c r="AL52" s="88"/>
+      <c r="AM52" s="88"/>
+      <c r="AN52" s="88"/>
+      <c r="AO52" s="88"/>
+      <c r="AP52" s="88"/>
+      <c r="AQ52" s="88"/>
+      <c r="AR52" s="88"/>
+      <c r="AS52" s="88"/>
+      <c r="AT52" s="88"/>
+      <c r="AU52" s="88"/>
+      <c r="AV52" s="88"/>
+      <c r="AW52" s="88"/>
+      <c r="AX52" s="88"/>
+      <c r="AY52" s="88"/>
+      <c r="AZ52" s="88"/>
+      <c r="BA52" s="88"/>
+      <c r="BB52" s="88"/>
+      <c r="BC52" s="88"/>
+      <c r="BD52" s="88"/>
+      <c r="BE52" s="88"/>
+      <c r="BF52" s="88"/>
+      <c r="BG52" s="88"/>
+      <c r="BH52" s="88"/>
+      <c r="BI52" s="88"/>
+      <c r="BJ52" s="88"/>
+      <c r="BK52" s="88"/>
+      <c r="BL52" s="88"/>
+      <c r="BM52" s="88"/>
+      <c r="BN52" s="88"/>
+      <c r="BO52" s="88"/>
+      <c r="BP52" s="88"/>
+      <c r="BQ52" s="88"/>
+      <c r="BR52" s="88"/>
+      <c r="BS52" s="88"/>
+      <c r="BT52" s="88"/>
+      <c r="BU52" s="88"/>
+      <c r="BV52" s="88"/>
+      <c r="BW52" s="88"/>
+      <c r="BX52" s="88"/>
+      <c r="BY52" s="88"/>
+      <c r="BZ52" s="88"/>
+    </row>
+    <row r="53" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="72"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="63"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="65"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="67"/>
-      <c r="L52" s="67"/>
-      <c r="M52" s="67"/>
-      <c r="N52" s="68"/>
-      <c r="O52" s="68"/>
-      <c r="P52" s="68"/>
-      <c r="Q52" s="68"/>
-      <c r="R52" s="68"/>
-      <c r="S52" s="67"/>
-      <c r="T52" s="67"/>
-      <c r="U52" s="67"/>
-      <c r="V52" s="67"/>
-      <c r="W52" s="67"/>
-      <c r="X52" s="67"/>
-      <c r="Y52" s="67"/>
-      <c r="Z52" s="67"/>
-      <c r="AA52" s="67"/>
-      <c r="AB52" s="67"/>
-      <c r="AC52" s="69"/>
-      <c r="AD52" s="69"/>
-      <c r="AE52" s="69"/>
-      <c r="AF52" s="69"/>
-      <c r="AG52" s="69"/>
-      <c r="AH52" s="67"/>
-      <c r="AI52" s="67"/>
-      <c r="AJ52" s="67"/>
-      <c r="AK52" s="67"/>
-      <c r="AL52" s="67"/>
-      <c r="AM52" s="67"/>
-      <c r="AN52" s="67"/>
-      <c r="AO52" s="67"/>
-      <c r="AP52" s="67"/>
-      <c r="AQ52" s="67"/>
-      <c r="AR52" s="70"/>
-      <c r="AS52" s="70"/>
-      <c r="AT52" s="70"/>
-      <c r="AU52" s="70"/>
-      <c r="AV52" s="70"/>
-      <c r="AW52" s="67"/>
-      <c r="AX52" s="67"/>
-      <c r="AY52" s="67"/>
-      <c r="AZ52" s="67"/>
-      <c r="BA52" s="67"/>
-      <c r="BB52" s="67"/>
-      <c r="BC52" s="67"/>
-      <c r="BD52" s="67"/>
-      <c r="BE52" s="67"/>
-      <c r="BF52" s="67"/>
-      <c r="BG52" s="71"/>
-      <c r="BH52" s="71"/>
-      <c r="BI52" s="71"/>
-      <c r="BJ52" s="71"/>
-      <c r="BK52" s="71"/>
-      <c r="BL52" s="67"/>
-      <c r="BM52" s="67"/>
-      <c r="BN52" s="67"/>
-      <c r="BO52" s="67"/>
-      <c r="BP52" s="67"/>
-      <c r="BQ52" s="67"/>
-      <c r="BR52" s="67"/>
-      <c r="BS52" s="67"/>
-      <c r="BT52" s="67"/>
-      <c r="BU52" s="67"/>
-      <c r="BV52" s="67"/>
-      <c r="BW52" s="67"/>
-      <c r="BX52" s="67"/>
-      <c r="BY52" s="67"/>
-      <c r="BZ52" s="67"/>
-    </row>
-    <row r="53" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" s="54"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="129"/>
-      <c r="J53" s="129"/>
-      <c r="K53" s="129"/>
-      <c r="L53" s="129"/>
-      <c r="M53" s="129"/>
-      <c r="N53" s="129"/>
-      <c r="O53" s="129"/>
-      <c r="P53" s="129"/>
-      <c r="Q53" s="129"/>
-      <c r="R53" s="129"/>
-      <c r="S53" s="129"/>
-      <c r="T53" s="129"/>
-      <c r="U53" s="129"/>
-      <c r="V53" s="129"/>
-      <c r="W53" s="129"/>
-      <c r="X53" s="129"/>
-      <c r="Y53" s="129"/>
-      <c r="Z53" s="129"/>
-      <c r="AA53" s="129"/>
-      <c r="AB53" s="129"/>
-      <c r="AC53" s="129"/>
-      <c r="AD53" s="129"/>
-      <c r="AE53" s="129"/>
-      <c r="AF53" s="129"/>
-      <c r="AG53" s="129"/>
-      <c r="AH53" s="38"/>
-      <c r="AI53" s="38"/>
-      <c r="AJ53" s="124"/>
-      <c r="AK53" s="124"/>
-      <c r="AL53" s="124"/>
-      <c r="AM53" s="58"/>
-      <c r="AN53" s="38"/>
-      <c r="AO53" s="38"/>
-      <c r="AP53" s="38"/>
-      <c r="AQ53" s="38"/>
-      <c r="AR53" s="40"/>
-      <c r="AS53" s="40"/>
-      <c r="AT53" s="40"/>
-      <c r="AU53" s="40"/>
-      <c r="AV53" s="40"/>
-      <c r="AW53" s="38"/>
-      <c r="AX53" s="38"/>
-      <c r="AY53" s="38"/>
-      <c r="AZ53" s="38"/>
-      <c r="BA53" s="38"/>
-      <c r="BB53" s="38"/>
-      <c r="BC53" s="38"/>
-      <c r="BD53" s="38"/>
-      <c r="BE53" s="38"/>
-      <c r="BF53" s="38"/>
-      <c r="BG53" s="41"/>
-      <c r="BH53" s="41"/>
-      <c r="BI53" s="41"/>
-      <c r="BJ53" s="41"/>
-      <c r="BK53" s="41"/>
-      <c r="BL53" s="38"/>
-      <c r="BM53" s="38"/>
-      <c r="BN53" s="38"/>
-      <c r="BO53" s="38"/>
-      <c r="BP53" s="38"/>
-      <c r="BQ53" s="38"/>
-      <c r="BR53" s="38"/>
-      <c r="BS53" s="38"/>
-      <c r="BT53" s="38"/>
-      <c r="BU53" s="38"/>
-      <c r="BV53" s="38"/>
-      <c r="BW53" s="38"/>
-      <c r="BX53" s="38"/>
-      <c r="BY53" s="38"/>
-      <c r="BZ53" s="38"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="64"/>
+      <c r="I53" s="65"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="67"/>
+      <c r="L53" s="67"/>
+      <c r="M53" s="67"/>
+      <c r="N53" s="68"/>
+      <c r="O53" s="68"/>
+      <c r="P53" s="68"/>
+      <c r="Q53" s="68"/>
+      <c r="R53" s="68"/>
+      <c r="S53" s="67"/>
+      <c r="T53" s="67"/>
+      <c r="U53" s="67"/>
+      <c r="V53" s="67"/>
+      <c r="W53" s="67"/>
+      <c r="X53" s="67"/>
+      <c r="Y53" s="67"/>
+      <c r="Z53" s="67"/>
+      <c r="AA53" s="67"/>
+      <c r="AB53" s="67"/>
+      <c r="AC53" s="69"/>
+      <c r="AD53" s="69"/>
+      <c r="AE53" s="69"/>
+      <c r="AF53" s="69"/>
+      <c r="AG53" s="69"/>
+      <c r="AH53" s="67"/>
+      <c r="AI53" s="67"/>
+      <c r="AJ53" s="67"/>
+      <c r="AK53" s="67"/>
+      <c r="AL53" s="67"/>
+      <c r="AM53" s="67"/>
+      <c r="AN53" s="67"/>
+      <c r="AO53" s="67"/>
+      <c r="AP53" s="67"/>
+      <c r="AQ53" s="67"/>
+      <c r="AR53" s="70"/>
+      <c r="AS53" s="70"/>
+      <c r="AT53" s="70"/>
+      <c r="AU53" s="70"/>
+      <c r="AV53" s="70"/>
+      <c r="AW53" s="67"/>
+      <c r="AX53" s="67"/>
+      <c r="AY53" s="67"/>
+      <c r="AZ53" s="67"/>
+      <c r="BA53" s="67"/>
+      <c r="BB53" s="67"/>
+      <c r="BC53" s="67"/>
+      <c r="BD53" s="67"/>
+      <c r="BE53" s="67"/>
+      <c r="BF53" s="67"/>
+      <c r="BG53" s="71"/>
+      <c r="BH53" s="71"/>
+      <c r="BI53" s="71"/>
+      <c r="BJ53" s="71"/>
+      <c r="BK53" s="71"/>
+      <c r="BL53" s="67"/>
+      <c r="BM53" s="67"/>
+      <c r="BN53" s="67"/>
+      <c r="BO53" s="67"/>
+      <c r="BP53" s="67"/>
+      <c r="BQ53" s="67"/>
+      <c r="BR53" s="67"/>
+      <c r="BS53" s="67"/>
+      <c r="BT53" s="67"/>
+      <c r="BU53" s="67"/>
+      <c r="BV53" s="67"/>
+      <c r="BW53" s="67"/>
+      <c r="BX53" s="67"/>
+      <c r="BY53" s="67"/>
+      <c r="BZ53" s="67"/>
     </row>
     <row r="54" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32"/>
@@ -6779,7 +6775,7 @@
       <c r="AK55" s="124"/>
       <c r="AL55" s="124"/>
       <c r="AM55" s="58"/>
-      <c r="AN55" s="131"/>
+      <c r="AN55" s="38"/>
       <c r="AO55" s="38"/>
       <c r="AP55" s="38"/>
       <c r="AQ55" s="38"/>
@@ -6823,7 +6819,7 @@
       <c r="A56" s="32"/>
       <c r="B56" s="53"/>
       <c r="C56" s="56" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="D56" s="54"/>
       <c r="E56" s="35"/>
@@ -6857,11 +6853,11 @@
       <c r="AG56" s="129"/>
       <c r="AH56" s="38"/>
       <c r="AI56" s="38"/>
-      <c r="AJ56" s="38"/>
-      <c r="AK56" s="38"/>
-      <c r="AL56" s="38"/>
-      <c r="AM56" s="38"/>
-      <c r="AN56" s="130"/>
+      <c r="AJ56" s="124"/>
+      <c r="AK56" s="124"/>
+      <c r="AL56" s="124"/>
+      <c r="AM56" s="58"/>
+      <c r="AN56" s="131"/>
       <c r="AO56" s="38"/>
       <c r="AP56" s="38"/>
       <c r="AQ56" s="38"/>
@@ -6905,7 +6901,7 @@
       <c r="A57" s="32"/>
       <c r="B57" s="53"/>
       <c r="C57" s="56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D57" s="54"/>
       <c r="E57" s="35"/>
@@ -6943,7 +6939,7 @@
       <c r="AK57" s="38"/>
       <c r="AL57" s="38"/>
       <c r="AM57" s="38"/>
-      <c r="AN57" s="38"/>
+      <c r="AN57" s="130"/>
       <c r="AO57" s="38"/>
       <c r="AP57" s="38"/>
       <c r="AQ57" s="38"/>
@@ -6987,7 +6983,7 @@
       <c r="A58" s="32"/>
       <c r="B58" s="53"/>
       <c r="C58" s="56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D58" s="54"/>
       <c r="E58" s="35"/>
@@ -7024,16 +7020,17 @@
       <c r="AJ58" s="38"/>
       <c r="AK58" s="38"/>
       <c r="AL58" s="38"/>
+      <c r="AM58" s="38"/>
       <c r="AN58" s="38"/>
       <c r="AO58" s="38"/>
       <c r="AP58" s="38"/>
       <c r="AQ58" s="38"/>
-      <c r="AR58" s="150"/>
-      <c r="AS58" s="150"/>
-      <c r="AT58" s="150"/>
-      <c r="AU58" s="150"/>
-      <c r="AV58" s="150"/>
-      <c r="AW58" s="58"/>
+      <c r="AR58" s="40"/>
+      <c r="AS58" s="40"/>
+      <c r="AT58" s="40"/>
+      <c r="AU58" s="40"/>
+      <c r="AV58" s="40"/>
+      <c r="AW58" s="38"/>
       <c r="AX58" s="38"/>
       <c r="AY58" s="38"/>
       <c r="AZ58" s="38"/>
@@ -7068,7 +7065,7 @@
       <c r="A59" s="32"/>
       <c r="B59" s="53"/>
       <c r="C59" s="56" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="D59" s="54"/>
       <c r="E59" s="35"/>
@@ -7105,17 +7102,16 @@
       <c r="AJ59" s="38"/>
       <c r="AK59" s="38"/>
       <c r="AL59" s="38"/>
-      <c r="AM59" s="38"/>
       <c r="AN59" s="38"/>
       <c r="AO59" s="38"/>
       <c r="AP59" s="38"/>
       <c r="AQ59" s="38"/>
-      <c r="AR59" s="40"/>
-      <c r="AS59" s="40"/>
-      <c r="AT59" s="40"/>
-      <c r="AU59" s="40"/>
-      <c r="AV59" s="40"/>
-      <c r="AW59" s="38"/>
+      <c r="AR59" s="150"/>
+      <c r="AS59" s="150"/>
+      <c r="AT59" s="150"/>
+      <c r="AU59" s="150"/>
+      <c r="AV59" s="150"/>
+      <c r="AW59" s="58"/>
       <c r="AX59" s="38"/>
       <c r="AY59" s="38"/>
       <c r="AZ59" s="38"/>
@@ -7150,38 +7146,38 @@
       <c r="A60" s="32"/>
       <c r="B60" s="53"/>
       <c r="C60" s="56" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D60" s="54"/>
       <c r="E60" s="35"/>
       <c r="F60" s="35"/>
       <c r="G60" s="36"/>
       <c r="H60" s="37"/>
-      <c r="I60" s="42"/>
-      <c r="J60" s="43"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="44"/>
-      <c r="O60" s="44"/>
-      <c r="P60" s="44"/>
-      <c r="Q60" s="44"/>
-      <c r="R60" s="44"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="38"/>
-      <c r="U60" s="38"/>
-      <c r="V60" s="38"/>
-      <c r="W60" s="38"/>
-      <c r="X60" s="38"/>
-      <c r="Y60" s="38"/>
-      <c r="Z60" s="38"/>
-      <c r="AA60" s="38"/>
-      <c r="AB60" s="38"/>
-      <c r="AC60" s="39"/>
-      <c r="AD60" s="39"/>
-      <c r="AE60" s="39"/>
-      <c r="AF60" s="39"/>
-      <c r="AG60" s="39"/>
+      <c r="I60" s="129"/>
+      <c r="J60" s="129"/>
+      <c r="K60" s="129"/>
+      <c r="L60" s="129"/>
+      <c r="M60" s="129"/>
+      <c r="N60" s="129"/>
+      <c r="O60" s="129"/>
+      <c r="P60" s="129"/>
+      <c r="Q60" s="129"/>
+      <c r="R60" s="129"/>
+      <c r="S60" s="129"/>
+      <c r="T60" s="129"/>
+      <c r="U60" s="129"/>
+      <c r="V60" s="129"/>
+      <c r="W60" s="129"/>
+      <c r="X60" s="129"/>
+      <c r="Y60" s="129"/>
+      <c r="Z60" s="129"/>
+      <c r="AA60" s="129"/>
+      <c r="AB60" s="129"/>
+      <c r="AC60" s="129"/>
+      <c r="AD60" s="129"/>
+      <c r="AE60" s="129"/>
+      <c r="AF60" s="129"/>
+      <c r="AG60" s="129"/>
       <c r="AH60" s="38"/>
       <c r="AI60" s="38"/>
       <c r="AJ60" s="38"/>
@@ -7232,7 +7228,7 @@
       <c r="A61" s="32"/>
       <c r="B61" s="53"/>
       <c r="C61" s="56" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="D61" s="54"/>
       <c r="E61" s="35"/>
@@ -7314,7 +7310,7 @@
       <c r="A62" s="32"/>
       <c r="B62" s="53"/>
       <c r="C62" s="56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D62" s="54"/>
       <c r="E62" s="35"/>
@@ -7396,7 +7392,7 @@
       <c r="A63" s="32"/>
       <c r="B63" s="53"/>
       <c r="C63" s="56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D63" s="54"/>
       <c r="E63" s="35"/>
@@ -7478,7 +7474,7 @@
       <c r="A64" s="32"/>
       <c r="B64" s="53"/>
       <c r="C64" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D64" s="54"/>
       <c r="E64" s="35"/>
@@ -7560,7 +7556,7 @@
       <c r="A65" s="32"/>
       <c r="B65" s="53"/>
       <c r="C65" s="56" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="D65" s="54"/>
       <c r="E65" s="35"/>
@@ -7604,12 +7600,12 @@
       <c r="AQ65" s="38"/>
       <c r="AR65" s="40"/>
       <c r="AS65" s="40"/>
-      <c r="AT65" s="124"/>
-      <c r="AU65" s="124"/>
-      <c r="AV65" s="124"/>
-      <c r="AW65" s="124"/>
-      <c r="AX65" s="124"/>
-      <c r="AY65" s="58"/>
+      <c r="AT65" s="40"/>
+      <c r="AU65" s="40"/>
+      <c r="AV65" s="40"/>
+      <c r="AW65" s="38"/>
+      <c r="AX65" s="38"/>
+      <c r="AY65" s="38"/>
       <c r="AZ65" s="38"/>
       <c r="BA65" s="38"/>
       <c r="BB65" s="38"/>
@@ -7641,7 +7637,9 @@
     <row r="66" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
       <c r="B66" s="53"/>
-      <c r="C66" s="56"/>
+      <c r="C66" s="56" t="s">
+        <v>125</v>
+      </c>
       <c r="D66" s="54"/>
       <c r="E66" s="35"/>
       <c r="F66" s="35"/>
@@ -7684,12 +7682,12 @@
       <c r="AQ66" s="38"/>
       <c r="AR66" s="40"/>
       <c r="AS66" s="40"/>
-      <c r="AT66" s="40"/>
-      <c r="AU66" s="40"/>
-      <c r="AV66" s="40"/>
-      <c r="AW66" s="38"/>
-      <c r="AX66" s="38"/>
-      <c r="AY66" s="38"/>
+      <c r="AT66" s="124"/>
+      <c r="AU66" s="124"/>
+      <c r="AV66" s="124"/>
+      <c r="AW66" s="124"/>
+      <c r="AX66" s="124"/>
+      <c r="AY66" s="58"/>
       <c r="AZ66" s="38"/>
       <c r="BA66" s="38"/>
       <c r="BB66" s="38"/>
@@ -7800,173 +7798,171 @@
     </row>
     <row r="68" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="32"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="D68" s="61"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="65"/>
-      <c r="J68" s="66"/>
-      <c r="K68" s="67"/>
-      <c r="L68" s="67"/>
-      <c r="M68" s="67"/>
-      <c r="N68" s="68"/>
-      <c r="O68" s="68"/>
-      <c r="P68" s="68"/>
-      <c r="Q68" s="68"/>
-      <c r="R68" s="68"/>
-      <c r="S68" s="67"/>
-      <c r="T68" s="67"/>
-      <c r="U68" s="67"/>
-      <c r="V68" s="67"/>
-      <c r="W68" s="67"/>
-      <c r="X68" s="67"/>
-      <c r="Y68" s="67"/>
-      <c r="Z68" s="67"/>
-      <c r="AA68" s="67"/>
-      <c r="AB68" s="67"/>
-      <c r="AC68" s="69"/>
-      <c r="AD68" s="69"/>
-      <c r="AE68" s="69"/>
-      <c r="AF68" s="69"/>
-      <c r="AG68" s="69"/>
-      <c r="AH68" s="67"/>
-      <c r="AI68" s="67"/>
-      <c r="AJ68" s="67"/>
-      <c r="AK68" s="67"/>
-      <c r="AL68" s="67"/>
-      <c r="AM68" s="67"/>
-      <c r="AN68" s="67"/>
-      <c r="AO68" s="67"/>
-      <c r="AP68" s="67"/>
-      <c r="AQ68" s="67"/>
-      <c r="AR68" s="70"/>
-      <c r="AS68" s="70"/>
-      <c r="AT68" s="70"/>
-      <c r="AU68" s="70"/>
-      <c r="AV68" s="70"/>
-      <c r="AW68" s="67"/>
-      <c r="AX68" s="67"/>
-      <c r="AY68" s="67"/>
-      <c r="AZ68" s="67"/>
-      <c r="BA68" s="67"/>
-      <c r="BB68" s="67"/>
-      <c r="BC68" s="67"/>
-      <c r="BD68" s="67"/>
-      <c r="BE68" s="67"/>
-      <c r="BF68" s="67"/>
-      <c r="BG68" s="71"/>
-      <c r="BH68" s="71"/>
-      <c r="BI68" s="71"/>
-      <c r="BJ68" s="71"/>
-      <c r="BK68" s="71"/>
-      <c r="BL68" s="67"/>
-      <c r="BM68" s="67"/>
-      <c r="BN68" s="67"/>
-      <c r="BO68" s="67"/>
-      <c r="BP68" s="67"/>
-      <c r="BQ68" s="67"/>
-      <c r="BR68" s="67"/>
-      <c r="BS68" s="67"/>
-      <c r="BT68" s="67"/>
-      <c r="BU68" s="67"/>
-      <c r="BV68" s="67"/>
-      <c r="BW68" s="67"/>
-      <c r="BX68" s="67"/>
-      <c r="BY68" s="67"/>
-      <c r="BZ68" s="67"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="42"/>
+      <c r="J68" s="43"/>
+      <c r="K68" s="38"/>
+      <c r="L68" s="38"/>
+      <c r="M68" s="38"/>
+      <c r="N68" s="44"/>
+      <c r="O68" s="44"/>
+      <c r="P68" s="44"/>
+      <c r="Q68" s="44"/>
+      <c r="R68" s="44"/>
+      <c r="S68" s="38"/>
+      <c r="T68" s="38"/>
+      <c r="U68" s="38"/>
+      <c r="V68" s="38"/>
+      <c r="W68" s="38"/>
+      <c r="X68" s="38"/>
+      <c r="Y68" s="38"/>
+      <c r="Z68" s="38"/>
+      <c r="AA68" s="38"/>
+      <c r="AB68" s="38"/>
+      <c r="AC68" s="39"/>
+      <c r="AD68" s="39"/>
+      <c r="AE68" s="39"/>
+      <c r="AF68" s="39"/>
+      <c r="AG68" s="39"/>
+      <c r="AH68" s="38"/>
+      <c r="AI68" s="38"/>
+      <c r="AJ68" s="38"/>
+      <c r="AK68" s="38"/>
+      <c r="AL68" s="38"/>
+      <c r="AM68" s="38"/>
+      <c r="AN68" s="38"/>
+      <c r="AO68" s="38"/>
+      <c r="AP68" s="38"/>
+      <c r="AQ68" s="38"/>
+      <c r="AR68" s="40"/>
+      <c r="AS68" s="40"/>
+      <c r="AT68" s="40"/>
+      <c r="AU68" s="40"/>
+      <c r="AV68" s="40"/>
+      <c r="AW68" s="38"/>
+      <c r="AX68" s="38"/>
+      <c r="AY68" s="38"/>
+      <c r="AZ68" s="38"/>
+      <c r="BA68" s="38"/>
+      <c r="BB68" s="38"/>
+      <c r="BC68" s="38"/>
+      <c r="BD68" s="38"/>
+      <c r="BE68" s="38"/>
+      <c r="BF68" s="38"/>
+      <c r="BG68" s="41"/>
+      <c r="BH68" s="41"/>
+      <c r="BI68" s="41"/>
+      <c r="BJ68" s="41"/>
+      <c r="BK68" s="41"/>
+      <c r="BL68" s="38"/>
+      <c r="BM68" s="38"/>
+      <c r="BN68" s="38"/>
+      <c r="BO68" s="38"/>
+      <c r="BP68" s="38"/>
+      <c r="BQ68" s="38"/>
+      <c r="BR68" s="38"/>
+      <c r="BS68" s="38"/>
+      <c r="BT68" s="38"/>
+      <c r="BU68" s="38"/>
+      <c r="BV68" s="38"/>
+      <c r="BW68" s="38"/>
+      <c r="BX68" s="38"/>
+      <c r="BY68" s="38"/>
+      <c r="BZ68" s="38"/>
     </row>
     <row r="69" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="32"/>
-      <c r="B69" s="53"/>
-      <c r="C69" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="D69" s="54"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="37"/>
-      <c r="I69" s="42"/>
-      <c r="J69" s="43"/>
-      <c r="K69" s="38"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="44"/>
-      <c r="O69" s="44"/>
-      <c r="P69" s="44"/>
-      <c r="Q69" s="44"/>
-      <c r="R69" s="44"/>
-      <c r="S69" s="38"/>
-      <c r="T69" s="38"/>
-      <c r="U69" s="38"/>
-      <c r="V69" s="38"/>
-      <c r="W69" s="38"/>
-      <c r="X69" s="38"/>
-      <c r="Y69" s="38"/>
-      <c r="Z69" s="38"/>
-      <c r="AA69" s="38"/>
-      <c r="AB69" s="38"/>
-      <c r="AC69" s="39"/>
-      <c r="AD69" s="39"/>
-      <c r="AE69" s="39"/>
-      <c r="AF69" s="39"/>
-      <c r="AG69" s="39"/>
-      <c r="AH69" s="38"/>
-      <c r="AI69" s="124"/>
-      <c r="AJ69" s="124"/>
-      <c r="AK69" s="124"/>
-      <c r="AL69" s="124"/>
-      <c r="AM69" s="58"/>
-      <c r="AN69" s="38"/>
-      <c r="AO69" s="38"/>
-      <c r="AP69" s="38"/>
-      <c r="AQ69" s="38"/>
-      <c r="AR69" s="40"/>
-      <c r="AS69" s="40"/>
-      <c r="AT69" s="40"/>
-      <c r="AU69" s="40"/>
-      <c r="AV69" s="40"/>
-      <c r="AW69" s="38"/>
-      <c r="AX69" s="38"/>
-      <c r="AY69" s="38"/>
-      <c r="AZ69" s="38"/>
-      <c r="BA69" s="38"/>
-      <c r="BB69" s="38"/>
-      <c r="BC69" s="38"/>
-      <c r="BD69" s="38"/>
-      <c r="BE69" s="38"/>
-      <c r="BF69" s="38"/>
-      <c r="BG69" s="41"/>
-      <c r="BH69" s="41"/>
-      <c r="BI69" s="41"/>
-      <c r="BJ69" s="41"/>
-      <c r="BK69" s="41"/>
-      <c r="BL69" s="38"/>
-      <c r="BM69" s="38"/>
-      <c r="BN69" s="38"/>
-      <c r="BO69" s="38"/>
-      <c r="BP69" s="38"/>
-      <c r="BQ69" s="38"/>
-      <c r="BR69" s="38"/>
-      <c r="BS69" s="38"/>
-      <c r="BT69" s="38"/>
-      <c r="BU69" s="38"/>
-      <c r="BV69" s="38"/>
-      <c r="BW69" s="38"/>
-      <c r="BX69" s="38"/>
-      <c r="BY69" s="38"/>
-      <c r="BZ69" s="38"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" s="61"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="64"/>
+      <c r="I69" s="65"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="67"/>
+      <c r="L69" s="67"/>
+      <c r="M69" s="67"/>
+      <c r="N69" s="68"/>
+      <c r="O69" s="68"/>
+      <c r="P69" s="68"/>
+      <c r="Q69" s="68"/>
+      <c r="R69" s="68"/>
+      <c r="S69" s="67"/>
+      <c r="T69" s="67"/>
+      <c r="U69" s="67"/>
+      <c r="V69" s="67"/>
+      <c r="W69" s="67"/>
+      <c r="X69" s="67"/>
+      <c r="Y69" s="67"/>
+      <c r="Z69" s="67"/>
+      <c r="AA69" s="67"/>
+      <c r="AB69" s="67"/>
+      <c r="AC69" s="69"/>
+      <c r="AD69" s="69"/>
+      <c r="AE69" s="69"/>
+      <c r="AF69" s="69"/>
+      <c r="AG69" s="69"/>
+      <c r="AH69" s="67"/>
+      <c r="AI69" s="67"/>
+      <c r="AJ69" s="67"/>
+      <c r="AK69" s="67"/>
+      <c r="AL69" s="67"/>
+      <c r="AM69" s="67"/>
+      <c r="AN69" s="67"/>
+      <c r="AO69" s="67"/>
+      <c r="AP69" s="67"/>
+      <c r="AQ69" s="67"/>
+      <c r="AR69" s="70"/>
+      <c r="AS69" s="70"/>
+      <c r="AT69" s="70"/>
+      <c r="AU69" s="70"/>
+      <c r="AV69" s="70"/>
+      <c r="AW69" s="67"/>
+      <c r="AX69" s="67"/>
+      <c r="AY69" s="67"/>
+      <c r="AZ69" s="67"/>
+      <c r="BA69" s="67"/>
+      <c r="BB69" s="67"/>
+      <c r="BC69" s="67"/>
+      <c r="BD69" s="67"/>
+      <c r="BE69" s="67"/>
+      <c r="BF69" s="67"/>
+      <c r="BG69" s="71"/>
+      <c r="BH69" s="71"/>
+      <c r="BI69" s="71"/>
+      <c r="BJ69" s="71"/>
+      <c r="BK69" s="71"/>
+      <c r="BL69" s="67"/>
+      <c r="BM69" s="67"/>
+      <c r="BN69" s="67"/>
+      <c r="BO69" s="67"/>
+      <c r="BP69" s="67"/>
+      <c r="BQ69" s="67"/>
+      <c r="BR69" s="67"/>
+      <c r="BS69" s="67"/>
+      <c r="BT69" s="67"/>
+      <c r="BU69" s="67"/>
+      <c r="BV69" s="67"/>
+      <c r="BW69" s="67"/>
+      <c r="BX69" s="67"/>
+      <c r="BY69" s="67"/>
+      <c r="BZ69" s="67"/>
     </row>
     <row r="70" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="32"/>
       <c r="B70" s="53"/>
       <c r="C70" s="56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D70" s="54"/>
       <c r="E70" s="35"/>
@@ -7993,11 +7989,11 @@
       <c r="Z70" s="38"/>
       <c r="AA70" s="38"/>
       <c r="AB70" s="38"/>
-      <c r="AC70" s="38"/>
-      <c r="AD70" s="38"/>
-      <c r="AE70" s="38"/>
-      <c r="AF70" s="38"/>
-      <c r="AG70" s="38"/>
+      <c r="AC70" s="39"/>
+      <c r="AD70" s="39"/>
+      <c r="AE70" s="39"/>
+      <c r="AF70" s="39"/>
+      <c r="AG70" s="39"/>
       <c r="AH70" s="38"/>
       <c r="AI70" s="124"/>
       <c r="AJ70" s="124"/>
@@ -8048,7 +8044,7 @@
       <c r="A71" s="32"/>
       <c r="B71" s="53"/>
       <c r="C71" s="56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D71" s="54"/>
       <c r="E71" s="35"/>
@@ -8130,7 +8126,7 @@
       <c r="A72" s="32"/>
       <c r="B72" s="53"/>
       <c r="C72" s="56" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D72" s="54"/>
       <c r="E72" s="35"/>
@@ -8157,11 +8153,11 @@
       <c r="Z72" s="38"/>
       <c r="AA72" s="38"/>
       <c r="AB72" s="38"/>
-      <c r="AC72" s="39"/>
-      <c r="AD72" s="39"/>
-      <c r="AE72" s="39"/>
-      <c r="AF72" s="39"/>
-      <c r="AG72" s="39"/>
+      <c r="AC72" s="38"/>
+      <c r="AD72" s="38"/>
+      <c r="AE72" s="38"/>
+      <c r="AF72" s="38"/>
+      <c r="AG72" s="38"/>
       <c r="AH72" s="38"/>
       <c r="AI72" s="124"/>
       <c r="AJ72" s="124"/>
@@ -8212,7 +8208,7 @@
       <c r="A73" s="32"/>
       <c r="B73" s="53"/>
       <c r="C73" s="56" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D73" s="54"/>
       <c r="E73" s="35"/>
@@ -8294,7 +8290,7 @@
       <c r="A74" s="32"/>
       <c r="B74" s="53"/>
       <c r="C74" s="56" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="D74" s="54"/>
       <c r="E74" s="35"/>
@@ -8327,11 +8323,11 @@
       <c r="AF74" s="39"/>
       <c r="AG74" s="39"/>
       <c r="AH74" s="38"/>
-      <c r="AI74" s="132"/>
-      <c r="AJ74" s="132"/>
-      <c r="AK74" s="132"/>
-      <c r="AL74" s="132"/>
-      <c r="AM74" s="133"/>
+      <c r="AI74" s="124"/>
+      <c r="AJ74" s="124"/>
+      <c r="AK74" s="124"/>
+      <c r="AL74" s="124"/>
+      <c r="AM74" s="58"/>
       <c r="AN74" s="38"/>
       <c r="AO74" s="38"/>
       <c r="AP74" s="38"/>
@@ -8376,7 +8372,7 @@
       <c r="A75" s="32"/>
       <c r="B75" s="53"/>
       <c r="C75" s="56" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D75" s="54"/>
       <c r="E75" s="35"/>
@@ -8409,17 +8405,17 @@
       <c r="AF75" s="39"/>
       <c r="AG75" s="39"/>
       <c r="AH75" s="38"/>
-      <c r="AI75" s="38"/>
-      <c r="AJ75" s="38"/>
-      <c r="AK75" s="38"/>
-      <c r="AL75" s="38"/>
-      <c r="AM75" s="38"/>
+      <c r="AI75" s="132"/>
+      <c r="AJ75" s="132"/>
+      <c r="AK75" s="132"/>
+      <c r="AL75" s="132"/>
+      <c r="AM75" s="133"/>
       <c r="AN75" s="38"/>
       <c r="AO75" s="38"/>
       <c r="AP75" s="38"/>
-      <c r="AQ75" s="124"/>
-      <c r="AR75" s="150"/>
-      <c r="AS75" s="147"/>
+      <c r="AQ75" s="38"/>
+      <c r="AR75" s="40"/>
+      <c r="AS75" s="40"/>
       <c r="AT75" s="40"/>
       <c r="AU75" s="40"/>
       <c r="AV75" s="40"/>
@@ -8458,7 +8454,7 @@
       <c r="A76" s="32"/>
       <c r="B76" s="53"/>
       <c r="C76" s="56" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D76" s="54"/>
       <c r="E76" s="35"/>
@@ -8499,13 +8495,13 @@
       <c r="AN76" s="38"/>
       <c r="AO76" s="38"/>
       <c r="AP76" s="38"/>
-      <c r="AQ76" s="38"/>
-      <c r="AR76" s="38"/>
-      <c r="AS76" s="40"/>
+      <c r="AQ76" s="124"/>
+      <c r="AR76" s="150"/>
+      <c r="AS76" s="147"/>
       <c r="AT76" s="40"/>
-      <c r="AU76" s="150"/>
-      <c r="AV76" s="150"/>
-      <c r="AW76" s="58"/>
+      <c r="AU76" s="40"/>
+      <c r="AV76" s="40"/>
+      <c r="AW76" s="38"/>
       <c r="AX76" s="38"/>
       <c r="AY76" s="38"/>
       <c r="AZ76" s="38"/>
@@ -8539,7 +8535,9 @@
     <row r="77" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="32"/>
       <c r="B77" s="53"/>
-      <c r="C77" s="56"/>
+      <c r="C77" s="56" t="s">
+        <v>126</v>
+      </c>
       <c r="D77" s="54"/>
       <c r="E77" s="35"/>
       <c r="F77" s="35"/>
@@ -8580,12 +8578,12 @@
       <c r="AO77" s="38"/>
       <c r="AP77" s="38"/>
       <c r="AQ77" s="38"/>
-      <c r="AR77" s="40"/>
+      <c r="AR77" s="38"/>
       <c r="AS77" s="40"/>
       <c r="AT77" s="40"/>
-      <c r="AU77" s="40"/>
-      <c r="AV77" s="40"/>
-      <c r="AW77" s="38"/>
+      <c r="AU77" s="150"/>
+      <c r="AV77" s="150"/>
+      <c r="AW77" s="58"/>
       <c r="AX77" s="38"/>
       <c r="AY77" s="38"/>
       <c r="AZ77" s="38"/>
@@ -8616,257 +8614,255 @@
       <c r="BY77" s="38"/>
       <c r="BZ77" s="38"/>
     </row>
-    <row r="78" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="72"/>
-      <c r="B78" s="59"/>
-      <c r="C78" s="60" t="s">
+    <row r="78" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="32"/>
+      <c r="B78" s="53"/>
+      <c r="C78" s="56"/>
+      <c r="D78" s="54"/>
+      <c r="E78" s="35"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="42"/>
+      <c r="J78" s="43"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="38"/>
+      <c r="M78" s="38"/>
+      <c r="N78" s="44"/>
+      <c r="O78" s="44"/>
+      <c r="P78" s="44"/>
+      <c r="Q78" s="44"/>
+      <c r="R78" s="44"/>
+      <c r="S78" s="38"/>
+      <c r="T78" s="38"/>
+      <c r="U78" s="38"/>
+      <c r="V78" s="38"/>
+      <c r="W78" s="38"/>
+      <c r="X78" s="38"/>
+      <c r="Y78" s="38"/>
+      <c r="Z78" s="38"/>
+      <c r="AA78" s="38"/>
+      <c r="AB78" s="38"/>
+      <c r="AC78" s="39"/>
+      <c r="AD78" s="39"/>
+      <c r="AE78" s="39"/>
+      <c r="AF78" s="39"/>
+      <c r="AG78" s="39"/>
+      <c r="AH78" s="38"/>
+      <c r="AI78" s="38"/>
+      <c r="AJ78" s="38"/>
+      <c r="AK78" s="38"/>
+      <c r="AL78" s="38"/>
+      <c r="AM78" s="38"/>
+      <c r="AN78" s="38"/>
+      <c r="AO78" s="38"/>
+      <c r="AP78" s="38"/>
+      <c r="AQ78" s="38"/>
+      <c r="AR78" s="40"/>
+      <c r="AS78" s="40"/>
+      <c r="AT78" s="40"/>
+      <c r="AU78" s="40"/>
+      <c r="AV78" s="40"/>
+      <c r="AW78" s="38"/>
+      <c r="AX78" s="38"/>
+      <c r="AY78" s="38"/>
+      <c r="AZ78" s="38"/>
+      <c r="BA78" s="38"/>
+      <c r="BB78" s="38"/>
+      <c r="BC78" s="38"/>
+      <c r="BD78" s="38"/>
+      <c r="BE78" s="38"/>
+      <c r="BF78" s="38"/>
+      <c r="BG78" s="41"/>
+      <c r="BH78" s="41"/>
+      <c r="BI78" s="41"/>
+      <c r="BJ78" s="41"/>
+      <c r="BK78" s="41"/>
+      <c r="BL78" s="38"/>
+      <c r="BM78" s="38"/>
+      <c r="BN78" s="38"/>
+      <c r="BO78" s="38"/>
+      <c r="BP78" s="38"/>
+      <c r="BQ78" s="38"/>
+      <c r="BR78" s="38"/>
+      <c r="BS78" s="38"/>
+      <c r="BT78" s="38"/>
+      <c r="BU78" s="38"/>
+      <c r="BV78" s="38"/>
+      <c r="BW78" s="38"/>
+      <c r="BX78" s="38"/>
+      <c r="BY78" s="38"/>
+      <c r="BZ78" s="38"/>
+    </row>
+    <row r="79" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="72"/>
+      <c r="B79" s="59"/>
+      <c r="C79" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D78" s="61"/>
-      <c r="E78" s="62"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="64"/>
-      <c r="I78" s="65"/>
-      <c r="J78" s="66"/>
-      <c r="K78" s="67"/>
-      <c r="L78" s="67"/>
-      <c r="M78" s="67"/>
-      <c r="N78" s="68"/>
-      <c r="O78" s="68"/>
-      <c r="P78" s="68"/>
-      <c r="Q78" s="68"/>
-      <c r="R78" s="68"/>
-      <c r="S78" s="67"/>
-      <c r="T78" s="67"/>
-      <c r="U78" s="67"/>
-      <c r="V78" s="67"/>
-      <c r="W78" s="67"/>
-      <c r="X78" s="67"/>
-      <c r="Y78" s="67"/>
-      <c r="Z78" s="67"/>
-      <c r="AA78" s="67"/>
-      <c r="AB78" s="67"/>
-      <c r="AC78" s="69"/>
-      <c r="AD78" s="69"/>
-      <c r="AE78" s="69"/>
-      <c r="AF78" s="69"/>
-      <c r="AG78" s="69"/>
-      <c r="AH78" s="67"/>
-      <c r="AI78" s="67"/>
-      <c r="AJ78" s="69"/>
-      <c r="AK78" s="67"/>
-      <c r="AL78" s="67"/>
-      <c r="AM78" s="67"/>
-      <c r="AN78" s="67"/>
-      <c r="AO78" s="67"/>
-      <c r="AP78" s="67"/>
-      <c r="AQ78" s="67"/>
-      <c r="AR78" s="70"/>
-      <c r="AS78" s="70"/>
-      <c r="AT78" s="70"/>
-      <c r="AU78" s="70"/>
-      <c r="AV78" s="70"/>
-      <c r="AW78" s="67"/>
-      <c r="AX78" s="67"/>
-      <c r="AY78" s="67"/>
-      <c r="AZ78" s="67"/>
-      <c r="BA78" s="67"/>
-      <c r="BB78" s="67"/>
-      <c r="BC78" s="67"/>
-      <c r="BD78" s="67"/>
-      <c r="BE78" s="67"/>
-      <c r="BF78" s="67"/>
-      <c r="BG78" s="71"/>
-      <c r="BH78" s="71"/>
-      <c r="BI78" s="71"/>
-      <c r="BJ78" s="71"/>
-      <c r="BK78" s="71"/>
-      <c r="BL78" s="67"/>
-      <c r="BM78" s="67"/>
-      <c r="BN78" s="67"/>
-      <c r="BO78" s="67"/>
-      <c r="BP78" s="67"/>
-      <c r="BQ78" s="67"/>
-      <c r="BR78" s="67"/>
-      <c r="BS78" s="67"/>
-      <c r="BT78" s="67"/>
-      <c r="BU78" s="67"/>
-      <c r="BV78" s="67"/>
-      <c r="BW78" s="67"/>
-      <c r="BX78" s="67"/>
-      <c r="BY78" s="67"/>
-      <c r="BZ78" s="67"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="62"/>
+      <c r="F79" s="62"/>
+      <c r="G79" s="63"/>
+      <c r="H79" s="64"/>
+      <c r="I79" s="65"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="67"/>
+      <c r="L79" s="67"/>
+      <c r="M79" s="67"/>
+      <c r="N79" s="68"/>
+      <c r="O79" s="68"/>
+      <c r="P79" s="68"/>
+      <c r="Q79" s="68"/>
+      <c r="R79" s="68"/>
+      <c r="S79" s="67"/>
+      <c r="T79" s="67"/>
+      <c r="U79" s="67"/>
+      <c r="V79" s="67"/>
+      <c r="W79" s="67"/>
+      <c r="X79" s="67"/>
+      <c r="Y79" s="67"/>
+      <c r="Z79" s="67"/>
+      <c r="AA79" s="67"/>
+      <c r="AB79" s="67"/>
+      <c r="AC79" s="69"/>
+      <c r="AD79" s="69"/>
+      <c r="AE79" s="69"/>
+      <c r="AF79" s="69"/>
+      <c r="AG79" s="69"/>
+      <c r="AH79" s="67"/>
+      <c r="AI79" s="67"/>
+      <c r="AJ79" s="69"/>
+      <c r="AK79" s="67"/>
+      <c r="AL79" s="67"/>
+      <c r="AM79" s="67"/>
+      <c r="AN79" s="67"/>
+      <c r="AO79" s="67"/>
+      <c r="AP79" s="67"/>
+      <c r="AQ79" s="67"/>
+      <c r="AR79" s="70"/>
+      <c r="AS79" s="70"/>
+      <c r="AT79" s="70"/>
+      <c r="AU79" s="70"/>
+      <c r="AV79" s="70"/>
+      <c r="AW79" s="67"/>
+      <c r="AX79" s="67"/>
+      <c r="AY79" s="67"/>
+      <c r="AZ79" s="67"/>
+      <c r="BA79" s="67"/>
+      <c r="BB79" s="67"/>
+      <c r="BC79" s="67"/>
+      <c r="BD79" s="67"/>
+      <c r="BE79" s="67"/>
+      <c r="BF79" s="67"/>
+      <c r="BG79" s="71"/>
+      <c r="BH79" s="71"/>
+      <c r="BI79" s="71"/>
+      <c r="BJ79" s="71"/>
+      <c r="BK79" s="71"/>
+      <c r="BL79" s="67"/>
+      <c r="BM79" s="67"/>
+      <c r="BN79" s="67"/>
+      <c r="BO79" s="67"/>
+      <c r="BP79" s="67"/>
+      <c r="BQ79" s="67"/>
+      <c r="BR79" s="67"/>
+      <c r="BS79" s="67"/>
+      <c r="BT79" s="67"/>
+      <c r="BU79" s="67"/>
+      <c r="BV79" s="67"/>
+      <c r="BW79" s="67"/>
+      <c r="BX79" s="67"/>
+      <c r="BY79" s="67"/>
+      <c r="BZ79" s="67"/>
     </row>
-    <row r="79" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="91"/>
-      <c r="B79" s="92"/>
-      <c r="C79" s="93" t="s">
+    <row r="80" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="91"/>
+      <c r="B80" s="92"/>
+      <c r="C80" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="94"/>
-      <c r="E79" s="95"/>
-      <c r="F79" s="95"/>
-      <c r="G79" s="96"/>
-      <c r="H79" s="97"/>
-      <c r="I79" s="98"/>
-      <c r="J79" s="99"/>
-      <c r="K79" s="100"/>
-      <c r="L79" s="100"/>
-      <c r="M79" s="100"/>
-      <c r="N79" s="101"/>
-      <c r="O79" s="101"/>
-      <c r="P79" s="101"/>
-      <c r="Q79" s="101"/>
-      <c r="R79" s="101"/>
-      <c r="S79" s="100"/>
-      <c r="T79" s="100"/>
-      <c r="U79" s="100"/>
-      <c r="V79" s="100"/>
-      <c r="W79" s="100"/>
-      <c r="X79" s="100"/>
-      <c r="Y79" s="100"/>
-      <c r="Z79" s="100"/>
-      <c r="AA79" s="100"/>
-      <c r="AB79" s="100"/>
-      <c r="AC79" s="102"/>
-      <c r="AD79" s="102"/>
-      <c r="AE79" s="102"/>
-      <c r="AF79" s="102"/>
-      <c r="AG79" s="102"/>
-      <c r="AH79" s="100"/>
-      <c r="AI79" s="100"/>
-      <c r="AJ79" s="102"/>
-      <c r="AK79" s="100"/>
-      <c r="AL79" s="100"/>
-      <c r="AM79" s="100"/>
-      <c r="AN79" s="100"/>
-      <c r="AO79" s="100"/>
-      <c r="AP79" s="100"/>
-      <c r="AQ79" s="100"/>
-      <c r="AR79" s="103"/>
-      <c r="AS79" s="103"/>
-      <c r="AT79" s="103"/>
-      <c r="AU79" s="103"/>
-      <c r="AV79" s="103"/>
-      <c r="AW79" s="100"/>
-      <c r="AX79" s="100"/>
-      <c r="AY79" s="100"/>
-      <c r="AZ79" s="100"/>
-      <c r="BA79" s="100"/>
-      <c r="BB79" s="100"/>
-      <c r="BC79" s="100"/>
-      <c r="BD79" s="100"/>
-      <c r="BE79" s="100"/>
-      <c r="BF79" s="100"/>
-      <c r="BG79" s="104"/>
-      <c r="BH79" s="104"/>
-      <c r="BI79" s="104"/>
-      <c r="BJ79" s="104"/>
-      <c r="BK79" s="104"/>
-      <c r="BL79" s="100"/>
-      <c r="BM79" s="100"/>
-      <c r="BN79" s="100"/>
-      <c r="BO79" s="100"/>
-      <c r="BP79" s="100"/>
-      <c r="BQ79" s="100"/>
-      <c r="BR79" s="100"/>
-      <c r="BS79" s="100"/>
-      <c r="BT79" s="100"/>
-      <c r="BU79" s="100"/>
-      <c r="BV79" s="100"/>
-      <c r="BW79" s="100"/>
-      <c r="BX79" s="100"/>
-      <c r="BY79" s="100"/>
-      <c r="BZ79" s="100"/>
-    </row>
-    <row r="80" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
-      <c r="B80" s="53"/>
-      <c r="C80" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="D80" s="54"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="37"/>
-      <c r="I80" s="42"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="38"/>
-      <c r="L80" s="38"/>
-      <c r="M80" s="38"/>
-      <c r="N80" s="44"/>
-      <c r="O80" s="44"/>
-      <c r="P80" s="44"/>
-      <c r="Q80" s="44"/>
-      <c r="R80" s="44"/>
-      <c r="S80" s="38"/>
-      <c r="T80" s="38"/>
-      <c r="U80" s="38"/>
-      <c r="V80" s="38"/>
-      <c r="W80" s="38"/>
-      <c r="X80" s="38"/>
-      <c r="Y80" s="38"/>
-      <c r="Z80" s="38"/>
-      <c r="AA80" s="38"/>
-      <c r="AB80" s="38"/>
-      <c r="AC80" s="38"/>
-      <c r="AD80" s="38"/>
-      <c r="AE80" s="38"/>
-      <c r="AF80" s="38"/>
-      <c r="AG80" s="38"/>
-      <c r="AH80" s="123"/>
-      <c r="AI80" s="123"/>
-      <c r="AJ80" s="123"/>
-      <c r="AK80" s="123"/>
-      <c r="AL80" s="123"/>
-      <c r="AM80" s="58"/>
-      <c r="AN80" s="38"/>
-      <c r="AO80" s="38"/>
-      <c r="AP80" s="38"/>
-      <c r="AQ80" s="38"/>
-      <c r="AR80" s="40"/>
-      <c r="AS80" s="40"/>
-      <c r="AT80" s="40"/>
-      <c r="AU80" s="40"/>
-      <c r="AV80" s="40"/>
-      <c r="AW80" s="38"/>
-      <c r="AX80" s="38"/>
-      <c r="AY80" s="38"/>
-      <c r="AZ80" s="38"/>
-      <c r="BA80" s="38"/>
-      <c r="BB80" s="38"/>
-      <c r="BC80" s="38"/>
-      <c r="BD80" s="38"/>
-      <c r="BE80" s="38"/>
-      <c r="BF80" s="38"/>
-      <c r="BG80" s="41"/>
-      <c r="BH80" s="41"/>
-      <c r="BI80" s="41"/>
-      <c r="BJ80" s="41"/>
-      <c r="BK80" s="41"/>
-      <c r="BL80" s="38"/>
-      <c r="BM80" s="38"/>
-      <c r="BN80" s="38"/>
-      <c r="BO80" s="38"/>
-      <c r="BP80" s="38"/>
-      <c r="BQ80" s="38"/>
-      <c r="BR80" s="38"/>
-      <c r="BS80" s="38"/>
-      <c r="BT80" s="38"/>
-      <c r="BU80" s="38"/>
-      <c r="BV80" s="38"/>
-      <c r="BW80" s="38"/>
-      <c r="BX80" s="38"/>
-      <c r="BY80" s="38"/>
-      <c r="BZ80" s="38"/>
+      <c r="D80" s="94"/>
+      <c r="E80" s="95"/>
+      <c r="F80" s="95"/>
+      <c r="G80" s="96"/>
+      <c r="H80" s="97"/>
+      <c r="I80" s="98"/>
+      <c r="J80" s="99"/>
+      <c r="K80" s="100"/>
+      <c r="L80" s="100"/>
+      <c r="M80" s="100"/>
+      <c r="N80" s="101"/>
+      <c r="O80" s="101"/>
+      <c r="P80" s="101"/>
+      <c r="Q80" s="101"/>
+      <c r="R80" s="101"/>
+      <c r="S80" s="100"/>
+      <c r="T80" s="100"/>
+      <c r="U80" s="100"/>
+      <c r="V80" s="100"/>
+      <c r="W80" s="100"/>
+      <c r="X80" s="100"/>
+      <c r="Y80" s="100"/>
+      <c r="Z80" s="100"/>
+      <c r="AA80" s="100"/>
+      <c r="AB80" s="100"/>
+      <c r="AC80" s="102"/>
+      <c r="AD80" s="102"/>
+      <c r="AE80" s="102"/>
+      <c r="AF80" s="102"/>
+      <c r="AG80" s="102"/>
+      <c r="AH80" s="100"/>
+      <c r="AI80" s="100"/>
+      <c r="AJ80" s="102"/>
+      <c r="AK80" s="100"/>
+      <c r="AL80" s="100"/>
+      <c r="AM80" s="100"/>
+      <c r="AN80" s="100"/>
+      <c r="AO80" s="100"/>
+      <c r="AP80" s="100"/>
+      <c r="AQ80" s="100"/>
+      <c r="AR80" s="103"/>
+      <c r="AS80" s="103"/>
+      <c r="AT80" s="103"/>
+      <c r="AU80" s="103"/>
+      <c r="AV80" s="103"/>
+      <c r="AW80" s="100"/>
+      <c r="AX80" s="100"/>
+      <c r="AY80" s="100"/>
+      <c r="AZ80" s="100"/>
+      <c r="BA80" s="100"/>
+      <c r="BB80" s="100"/>
+      <c r="BC80" s="100"/>
+      <c r="BD80" s="100"/>
+      <c r="BE80" s="100"/>
+      <c r="BF80" s="100"/>
+      <c r="BG80" s="104"/>
+      <c r="BH80" s="104"/>
+      <c r="BI80" s="104"/>
+      <c r="BJ80" s="104"/>
+      <c r="BK80" s="104"/>
+      <c r="BL80" s="100"/>
+      <c r="BM80" s="100"/>
+      <c r="BN80" s="100"/>
+      <c r="BO80" s="100"/>
+      <c r="BP80" s="100"/>
+      <c r="BQ80" s="100"/>
+      <c r="BR80" s="100"/>
+      <c r="BS80" s="100"/>
+      <c r="BT80" s="100"/>
+      <c r="BU80" s="100"/>
+      <c r="BV80" s="100"/>
+      <c r="BW80" s="100"/>
+      <c r="BX80" s="100"/>
+      <c r="BY80" s="100"/>
+      <c r="BZ80" s="100"/>
     </row>
     <row r="81" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="32"/>
       <c r="B81" s="53"/>
       <c r="C81" s="56" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="D81" s="54"/>
       <c r="E81" s="35"/>
@@ -8898,12 +8894,12 @@
       <c r="AE81" s="38"/>
       <c r="AF81" s="38"/>
       <c r="AG81" s="38"/>
-      <c r="AH81" s="38"/>
-      <c r="AI81" s="38"/>
-      <c r="AJ81" s="38"/>
-      <c r="AK81" s="38"/>
-      <c r="AL81" s="38"/>
-      <c r="AM81" s="38"/>
+      <c r="AH81" s="123"/>
+      <c r="AI81" s="123"/>
+      <c r="AJ81" s="123"/>
+      <c r="AK81" s="123"/>
+      <c r="AL81" s="123"/>
+      <c r="AM81" s="58"/>
       <c r="AN81" s="38"/>
       <c r="AO81" s="38"/>
       <c r="AP81" s="38"/>
@@ -8948,7 +8944,7 @@
       <c r="A82" s="32"/>
       <c r="B82" s="53"/>
       <c r="C82" s="56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D82" s="54"/>
       <c r="E82" s="35"/>
@@ -8992,9 +8988,9 @@
       <c r="AQ82" s="38"/>
       <c r="AR82" s="40"/>
       <c r="AS82" s="40"/>
-      <c r="AT82" s="150"/>
-      <c r="AU82" s="150"/>
-      <c r="AV82" s="147"/>
+      <c r="AT82" s="40"/>
+      <c r="AU82" s="40"/>
+      <c r="AV82" s="40"/>
       <c r="AW82" s="38"/>
       <c r="AX82" s="38"/>
       <c r="AY82" s="38"/>
@@ -9026,11 +9022,11 @@
       <c r="BY82" s="38"/>
       <c r="BZ82" s="38"/>
     </row>
-    <row r="83" spans="1:78" ht="16.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="32"/>
       <c r="B83" s="53"/>
       <c r="C83" s="56" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="D83" s="54"/>
       <c r="E83" s="35"/>
@@ -9065,18 +9061,18 @@
       <c r="AH83" s="38"/>
       <c r="AI83" s="38"/>
       <c r="AJ83" s="38"/>
-      <c r="AK83" s="123"/>
-      <c r="AL83" s="123"/>
-      <c r="AM83" s="58"/>
+      <c r="AK83" s="38"/>
+      <c r="AL83" s="38"/>
+      <c r="AM83" s="38"/>
       <c r="AN83" s="38"/>
       <c r="AO83" s="38"/>
       <c r="AP83" s="38"/>
       <c r="AQ83" s="38"/>
       <c r="AR83" s="40"/>
       <c r="AS83" s="40"/>
-      <c r="AT83" s="40"/>
-      <c r="AU83" s="40"/>
-      <c r="AV83" s="40"/>
+      <c r="AT83" s="150"/>
+      <c r="AU83" s="150"/>
+      <c r="AV83" s="147"/>
       <c r="AW83" s="38"/>
       <c r="AX83" s="38"/>
       <c r="AY83" s="38"/>
@@ -9108,11 +9104,11 @@
       <c r="BY83" s="38"/>
       <c r="BZ83" s="38"/>
     </row>
-    <row r="84" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:78" ht="16.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="32"/>
       <c r="B84" s="53"/>
       <c r="C84" s="56" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="D84" s="54"/>
       <c r="E84" s="35"/>
@@ -9194,7 +9190,7 @@
       <c r="A85" s="32"/>
       <c r="B85" s="53"/>
       <c r="C85" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D85" s="54"/>
       <c r="E85" s="35"/>
@@ -9276,7 +9272,7 @@
       <c r="A86" s="32"/>
       <c r="B86" s="53"/>
       <c r="C86" s="56" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D86" s="54"/>
       <c r="E86" s="35"/>
@@ -9311,19 +9307,19 @@
       <c r="AH86" s="38"/>
       <c r="AI86" s="38"/>
       <c r="AJ86" s="38"/>
-      <c r="AK86" s="38"/>
-      <c r="AL86" s="38"/>
-      <c r="AM86" s="38"/>
+      <c r="AK86" s="123"/>
+      <c r="AL86" s="123"/>
+      <c r="AM86" s="58"/>
       <c r="AN86" s="38"/>
-      <c r="AO86" s="124"/>
-      <c r="AP86" s="124"/>
-      <c r="AQ86" s="124"/>
-      <c r="AR86" s="150"/>
-      <c r="AS86" s="150"/>
-      <c r="AT86" s="150"/>
-      <c r="AU86" s="150"/>
-      <c r="AV86" s="150"/>
-      <c r="AW86" s="58"/>
+      <c r="AO86" s="38"/>
+      <c r="AP86" s="38"/>
+      <c r="AQ86" s="38"/>
+      <c r="AR86" s="40"/>
+      <c r="AS86" s="40"/>
+      <c r="AT86" s="40"/>
+      <c r="AU86" s="40"/>
+      <c r="AV86" s="40"/>
+      <c r="AW86" s="38"/>
       <c r="AX86" s="38"/>
       <c r="AY86" s="38"/>
       <c r="AZ86" s="38"/>
@@ -9400,12 +9396,12 @@
       <c r="AO87" s="124"/>
       <c r="AP87" s="124"/>
       <c r="AQ87" s="124"/>
-      <c r="AR87" s="147"/>
-      <c r="AS87" s="40"/>
-      <c r="AT87" s="40"/>
-      <c r="AU87" s="40"/>
-      <c r="AV87" s="40"/>
-      <c r="AW87" s="38"/>
+      <c r="AR87" s="150"/>
+      <c r="AS87" s="150"/>
+      <c r="AT87" s="150"/>
+      <c r="AU87" s="150"/>
+      <c r="AV87" s="150"/>
+      <c r="AW87" s="58"/>
       <c r="AX87" s="38"/>
       <c r="AY87" s="38"/>
       <c r="AZ87" s="38"/>
@@ -9439,8 +9435,8 @@
     <row r="88" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="32"/>
       <c r="B88" s="53"/>
-      <c r="C88" s="57" t="s">
-        <v>130</v>
+      <c r="C88" s="56" t="s">
+        <v>119</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="35"/>
@@ -9479,9 +9475,9 @@
       <c r="AL88" s="38"/>
       <c r="AM88" s="38"/>
       <c r="AN88" s="38"/>
-      <c r="AO88" s="38"/>
-      <c r="AP88" s="38"/>
-      <c r="AQ88" s="38"/>
+      <c r="AO88" s="124"/>
+      <c r="AP88" s="124"/>
+      <c r="AQ88" s="124"/>
       <c r="AR88" s="147"/>
       <c r="AS88" s="40"/>
       <c r="AT88" s="40"/>
@@ -9521,8 +9517,8 @@
     <row r="89" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="32"/>
       <c r="B89" s="53"/>
-      <c r="C89" s="56" t="s">
-        <v>129</v>
+      <c r="C89" s="57" t="s">
+        <v>128</v>
       </c>
       <c r="D89" s="54"/>
       <c r="E89" s="35"/>
@@ -9549,11 +9545,11 @@
       <c r="Z89" s="38"/>
       <c r="AA89" s="38"/>
       <c r="AB89" s="38"/>
-      <c r="AC89" s="39"/>
-      <c r="AD89" s="39"/>
-      <c r="AE89" s="39"/>
-      <c r="AF89" s="39"/>
-      <c r="AG89" s="39"/>
+      <c r="AC89" s="38"/>
+      <c r="AD89" s="38"/>
+      <c r="AE89" s="38"/>
+      <c r="AF89" s="38"/>
+      <c r="AG89" s="38"/>
       <c r="AH89" s="38"/>
       <c r="AI89" s="38"/>
       <c r="AJ89" s="38"/>
@@ -9564,11 +9560,11 @@
       <c r="AO89" s="38"/>
       <c r="AP89" s="38"/>
       <c r="AQ89" s="38"/>
-      <c r="AR89" s="150"/>
-      <c r="AS89" s="150"/>
-      <c r="AT89" s="150"/>
-      <c r="AU89" s="150"/>
-      <c r="AV89" s="147"/>
+      <c r="AR89" s="147"/>
+      <c r="AS89" s="40"/>
+      <c r="AT89" s="40"/>
+      <c r="AU89" s="40"/>
+      <c r="AV89" s="40"/>
       <c r="AW89" s="38"/>
       <c r="AX89" s="38"/>
       <c r="AY89" s="38"/>
@@ -9604,7 +9600,7 @@
       <c r="A90" s="32"/>
       <c r="B90" s="53"/>
       <c r="C90" s="56" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
       <c r="D90" s="54"/>
       <c r="E90" s="35"/>
@@ -9686,7 +9682,7 @@
       <c r="A91" s="32"/>
       <c r="B91" s="53"/>
       <c r="C91" s="56" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="D91" s="54"/>
       <c r="E91" s="35"/>
@@ -9768,7 +9764,7 @@
       <c r="A92" s="32"/>
       <c r="B92" s="53"/>
       <c r="C92" s="56" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D92" s="54"/>
       <c r="E92" s="35"/>
@@ -9846,175 +9842,175 @@
       <c r="BY92" s="38"/>
       <c r="BZ92" s="38"/>
     </row>
-    <row r="93" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="91"/>
-      <c r="B93" s="92"/>
-      <c r="C93" s="93" t="s">
+    <row r="93" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="32"/>
+      <c r="B93" s="53"/>
+      <c r="C93" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D93" s="54"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="42"/>
+      <c r="J93" s="43"/>
+      <c r="K93" s="38"/>
+      <c r="L93" s="38"/>
+      <c r="M93" s="38"/>
+      <c r="N93" s="44"/>
+      <c r="O93" s="44"/>
+      <c r="P93" s="44"/>
+      <c r="Q93" s="44"/>
+      <c r="R93" s="44"/>
+      <c r="S93" s="38"/>
+      <c r="T93" s="38"/>
+      <c r="U93" s="38"/>
+      <c r="V93" s="38"/>
+      <c r="W93" s="38"/>
+      <c r="X93" s="38"/>
+      <c r="Y93" s="38"/>
+      <c r="Z93" s="38"/>
+      <c r="AA93" s="38"/>
+      <c r="AB93" s="38"/>
+      <c r="AC93" s="39"/>
+      <c r="AD93" s="39"/>
+      <c r="AE93" s="39"/>
+      <c r="AF93" s="39"/>
+      <c r="AG93" s="39"/>
+      <c r="AH93" s="38"/>
+      <c r="AI93" s="38"/>
+      <c r="AJ93" s="38"/>
+      <c r="AK93" s="38"/>
+      <c r="AL93" s="38"/>
+      <c r="AM93" s="38"/>
+      <c r="AN93" s="38"/>
+      <c r="AO93" s="38"/>
+      <c r="AP93" s="38"/>
+      <c r="AQ93" s="38"/>
+      <c r="AR93" s="150"/>
+      <c r="AS93" s="150"/>
+      <c r="AT93" s="150"/>
+      <c r="AU93" s="150"/>
+      <c r="AV93" s="147"/>
+      <c r="AW93" s="38"/>
+      <c r="AX93" s="38"/>
+      <c r="AY93" s="38"/>
+      <c r="AZ93" s="38"/>
+      <c r="BA93" s="38"/>
+      <c r="BB93" s="38"/>
+      <c r="BC93" s="38"/>
+      <c r="BD93" s="38"/>
+      <c r="BE93" s="38"/>
+      <c r="BF93" s="38"/>
+      <c r="BG93" s="41"/>
+      <c r="BH93" s="41"/>
+      <c r="BI93" s="41"/>
+      <c r="BJ93" s="41"/>
+      <c r="BK93" s="41"/>
+      <c r="BL93" s="38"/>
+      <c r="BM93" s="38"/>
+      <c r="BN93" s="38"/>
+      <c r="BO93" s="38"/>
+      <c r="BP93" s="38"/>
+      <c r="BQ93" s="38"/>
+      <c r="BR93" s="38"/>
+      <c r="BS93" s="38"/>
+      <c r="BT93" s="38"/>
+      <c r="BU93" s="38"/>
+      <c r="BV93" s="38"/>
+      <c r="BW93" s="38"/>
+      <c r="BX93" s="38"/>
+      <c r="BY93" s="38"/>
+      <c r="BZ93" s="38"/>
+    </row>
+    <row r="94" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="91"/>
+      <c r="B94" s="92"/>
+      <c r="C94" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="D93" s="94"/>
-      <c r="E93" s="95"/>
-      <c r="F93" s="95"/>
-      <c r="G93" s="96"/>
-      <c r="H93" s="97"/>
-      <c r="I93" s="98"/>
-      <c r="J93" s="99"/>
-      <c r="K93" s="100"/>
-      <c r="L93" s="100"/>
-      <c r="M93" s="100"/>
-      <c r="N93" s="101"/>
-      <c r="O93" s="101"/>
-      <c r="P93" s="101"/>
-      <c r="Q93" s="101"/>
-      <c r="R93" s="101"/>
-      <c r="S93" s="100"/>
-      <c r="T93" s="100"/>
-      <c r="U93" s="100"/>
-      <c r="V93" s="100"/>
-      <c r="W93" s="100"/>
-      <c r="X93" s="100"/>
-      <c r="Y93" s="100"/>
-      <c r="Z93" s="100"/>
-      <c r="AA93" s="100"/>
-      <c r="AB93" s="100"/>
-      <c r="AC93" s="102"/>
-      <c r="AD93" s="102"/>
-      <c r="AE93" s="102"/>
-      <c r="AF93" s="102"/>
-      <c r="AG93" s="102"/>
-      <c r="AH93" s="100"/>
-      <c r="AI93" s="100"/>
-      <c r="AJ93" s="100"/>
-      <c r="AK93" s="100"/>
-      <c r="AL93" s="100"/>
-      <c r="AM93" s="100"/>
-      <c r="AN93" s="100"/>
-      <c r="AO93" s="100"/>
-      <c r="AP93" s="100"/>
-      <c r="AQ93" s="100"/>
-      <c r="AR93" s="103"/>
-      <c r="AS93" s="103"/>
-      <c r="AT93" s="103"/>
-      <c r="AU93" s="103"/>
-      <c r="AV93" s="103"/>
-      <c r="AW93" s="100"/>
-      <c r="AX93" s="100"/>
-      <c r="AY93" s="100"/>
-      <c r="AZ93" s="100"/>
-      <c r="BA93" s="100"/>
-      <c r="BB93" s="100"/>
-      <c r="BC93" s="100"/>
-      <c r="BD93" s="100"/>
-      <c r="BE93" s="100"/>
-      <c r="BF93" s="100"/>
-      <c r="BG93" s="104"/>
-      <c r="BH93" s="104"/>
-      <c r="BI93" s="104"/>
-      <c r="BJ93" s="104"/>
-      <c r="BK93" s="104"/>
-      <c r="BL93" s="100"/>
-      <c r="BM93" s="100"/>
-      <c r="BN93" s="100"/>
-      <c r="BO93" s="100"/>
-      <c r="BP93" s="100"/>
-      <c r="BQ93" s="100"/>
-      <c r="BR93" s="100"/>
-      <c r="BS93" s="100"/>
-      <c r="BT93" s="100"/>
-      <c r="BU93" s="100"/>
-      <c r="BV93" s="100"/>
-      <c r="BW93" s="100"/>
-      <c r="BX93" s="100"/>
-      <c r="BY93" s="100"/>
-      <c r="BZ93" s="100"/>
-    </row>
-    <row r="94" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="32"/>
-      <c r="B94" s="53"/>
-      <c r="C94" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="D94" s="54"/>
-      <c r="E94" s="35"/>
-      <c r="F94" s="35"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="37"/>
-      <c r="I94" s="42"/>
-      <c r="J94" s="43"/>
-      <c r="K94" s="38"/>
-      <c r="L94" s="38"/>
-      <c r="M94" s="38"/>
-      <c r="N94" s="38"/>
-      <c r="O94" s="38"/>
-      <c r="P94" s="38"/>
-      <c r="Q94" s="38"/>
-      <c r="R94" s="38"/>
-      <c r="S94" s="38"/>
-      <c r="T94" s="38"/>
-      <c r="U94" s="38"/>
-      <c r="V94" s="38"/>
-      <c r="W94" s="38"/>
-      <c r="X94" s="38"/>
-      <c r="Y94" s="38"/>
-      <c r="Z94" s="38"/>
-      <c r="AA94" s="38"/>
-      <c r="AB94" s="38"/>
-      <c r="AC94" s="38"/>
-      <c r="AD94" s="38"/>
-      <c r="AE94" s="38"/>
-      <c r="AF94" s="38"/>
-      <c r="AG94" s="38"/>
-      <c r="AH94" s="38"/>
-      <c r="AI94" s="124"/>
-      <c r="AJ94" s="124"/>
-      <c r="AK94" s="124"/>
-      <c r="AL94" s="124"/>
-      <c r="AM94" s="58"/>
-      <c r="AN94" s="38"/>
-      <c r="AO94" s="38"/>
-      <c r="AP94" s="38"/>
-      <c r="AQ94" s="38"/>
-      <c r="AR94" s="38"/>
-      <c r="AS94" s="38"/>
-      <c r="AT94" s="38"/>
-      <c r="AU94" s="38"/>
-      <c r="AV94" s="38"/>
-      <c r="AW94" s="38"/>
-      <c r="AX94" s="38"/>
-      <c r="AY94" s="38"/>
-      <c r="AZ94" s="38"/>
-      <c r="BA94" s="38"/>
-      <c r="BB94" s="38"/>
-      <c r="BC94" s="38"/>
-      <c r="BD94" s="38"/>
-      <c r="BE94" s="38"/>
-      <c r="BF94" s="38"/>
-      <c r="BG94" s="38"/>
-      <c r="BH94" s="38"/>
-      <c r="BI94" s="38"/>
-      <c r="BJ94" s="38"/>
-      <c r="BK94" s="38"/>
-      <c r="BL94" s="38"/>
-      <c r="BM94" s="38"/>
-      <c r="BN94" s="38"/>
-      <c r="BO94" s="38"/>
-      <c r="BP94" s="38"/>
-      <c r="BQ94" s="38"/>
-      <c r="BR94" s="38"/>
-      <c r="BS94" s="38"/>
-      <c r="BT94" s="38"/>
-      <c r="BU94" s="38"/>
-      <c r="BV94" s="38"/>
-      <c r="BW94" s="38"/>
-      <c r="BX94" s="38"/>
-      <c r="BY94" s="38"/>
-      <c r="BZ94" s="38"/>
+      <c r="D94" s="94"/>
+      <c r="E94" s="95"/>
+      <c r="F94" s="95"/>
+      <c r="G94" s="96"/>
+      <c r="H94" s="97"/>
+      <c r="I94" s="98"/>
+      <c r="J94" s="99"/>
+      <c r="K94" s="100"/>
+      <c r="L94" s="100"/>
+      <c r="M94" s="100"/>
+      <c r="N94" s="101"/>
+      <c r="O94" s="101"/>
+      <c r="P94" s="101"/>
+      <c r="Q94" s="101"/>
+      <c r="R94" s="101"/>
+      <c r="S94" s="100"/>
+      <c r="T94" s="100"/>
+      <c r="U94" s="100"/>
+      <c r="V94" s="100"/>
+      <c r="W94" s="100"/>
+      <c r="X94" s="100"/>
+      <c r="Y94" s="100"/>
+      <c r="Z94" s="100"/>
+      <c r="AA94" s="100"/>
+      <c r="AB94" s="100"/>
+      <c r="AC94" s="102"/>
+      <c r="AD94" s="102"/>
+      <c r="AE94" s="102"/>
+      <c r="AF94" s="102"/>
+      <c r="AG94" s="102"/>
+      <c r="AH94" s="100"/>
+      <c r="AI94" s="100"/>
+      <c r="AJ94" s="100"/>
+      <c r="AK94" s="100"/>
+      <c r="AL94" s="100"/>
+      <c r="AM94" s="100"/>
+      <c r="AN94" s="100"/>
+      <c r="AO94" s="100"/>
+      <c r="AP94" s="100"/>
+      <c r="AQ94" s="100"/>
+      <c r="AR94" s="103"/>
+      <c r="AS94" s="103"/>
+      <c r="AT94" s="103"/>
+      <c r="AU94" s="103"/>
+      <c r="AV94" s="103"/>
+      <c r="AW94" s="100"/>
+      <c r="AX94" s="100"/>
+      <c r="AY94" s="100"/>
+      <c r="AZ94" s="100"/>
+      <c r="BA94" s="100"/>
+      <c r="BB94" s="100"/>
+      <c r="BC94" s="100"/>
+      <c r="BD94" s="100"/>
+      <c r="BE94" s="100"/>
+      <c r="BF94" s="100"/>
+      <c r="BG94" s="104"/>
+      <c r="BH94" s="104"/>
+      <c r="BI94" s="104"/>
+      <c r="BJ94" s="104"/>
+      <c r="BK94" s="104"/>
+      <c r="BL94" s="100"/>
+      <c r="BM94" s="100"/>
+      <c r="BN94" s="100"/>
+      <c r="BO94" s="100"/>
+      <c r="BP94" s="100"/>
+      <c r="BQ94" s="100"/>
+      <c r="BR94" s="100"/>
+      <c r="BS94" s="100"/>
+      <c r="BT94" s="100"/>
+      <c r="BU94" s="100"/>
+      <c r="BV94" s="100"/>
+      <c r="BW94" s="100"/>
+      <c r="BX94" s="100"/>
+      <c r="BY94" s="100"/>
+      <c r="BZ94" s="100"/>
     </row>
     <row r="95" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="32"/>
       <c r="B95" s="53"/>
       <c r="C95" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D95" s="54"/>
       <c r="E95" s="35"/>
@@ -10047,11 +10043,11 @@
       <c r="AF95" s="38"/>
       <c r="AG95" s="38"/>
       <c r="AH95" s="38"/>
-      <c r="AI95" s="38"/>
-      <c r="AJ95" s="38"/>
-      <c r="AK95" s="38"/>
-      <c r="AL95" s="38"/>
-      <c r="AM95" s="38"/>
+      <c r="AI95" s="124"/>
+      <c r="AJ95" s="124"/>
+      <c r="AK95" s="124"/>
+      <c r="AL95" s="124"/>
+      <c r="AM95" s="58"/>
       <c r="AN95" s="38"/>
       <c r="AO95" s="38"/>
       <c r="AP95" s="38"/>
@@ -10096,7 +10092,7 @@
       <c r="A96" s="32"/>
       <c r="B96" s="53"/>
       <c r="C96" s="56" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="D96" s="54"/>
       <c r="E96" s="35"/>
@@ -10138,12 +10134,12 @@
       <c r="AO96" s="38"/>
       <c r="AP96" s="38"/>
       <c r="AQ96" s="38"/>
-      <c r="AR96" s="124"/>
-      <c r="AS96" s="124"/>
-      <c r="AT96" s="124"/>
-      <c r="AU96" s="124"/>
-      <c r="AV96" s="124"/>
-      <c r="AW96" s="58"/>
+      <c r="AR96" s="38"/>
+      <c r="AS96" s="38"/>
+      <c r="AT96" s="38"/>
+      <c r="AU96" s="38"/>
+      <c r="AV96" s="38"/>
+      <c r="AW96" s="38"/>
       <c r="AX96" s="38"/>
       <c r="AY96" s="38"/>
       <c r="AZ96" s="38"/>
@@ -10177,7 +10173,9 @@
     <row r="97" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="32"/>
       <c r="B97" s="53"/>
-      <c r="C97" s="56"/>
+      <c r="C97" s="56" t="s">
+        <v>129</v>
+      </c>
       <c r="D97" s="54"/>
       <c r="E97" s="35"/>
       <c r="F97" s="35"/>
@@ -10218,12 +10216,12 @@
       <c r="AO97" s="38"/>
       <c r="AP97" s="38"/>
       <c r="AQ97" s="38"/>
-      <c r="AR97" s="38"/>
-      <c r="AS97" s="38"/>
-      <c r="AT97" s="38"/>
-      <c r="AU97" s="38"/>
-      <c r="AV97" s="38"/>
-      <c r="AW97" s="38"/>
+      <c r="AR97" s="124"/>
+      <c r="AS97" s="124"/>
+      <c r="AT97" s="124"/>
+      <c r="AU97" s="124"/>
+      <c r="AV97" s="124"/>
+      <c r="AW97" s="58"/>
       <c r="AX97" s="38"/>
       <c r="AY97" s="38"/>
       <c r="AZ97" s="38"/>
@@ -10254,175 +10252,173 @@
       <c r="BY97" s="38"/>
       <c r="BZ97" s="38"/>
     </row>
-    <row r="98" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="72"/>
-      <c r="B98" s="59"/>
-      <c r="C98" s="77" t="s">
+    <row r="98" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="32"/>
+      <c r="B98" s="53"/>
+      <c r="C98" s="56"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="35"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="42"/>
+      <c r="J98" s="43"/>
+      <c r="K98" s="38"/>
+      <c r="L98" s="38"/>
+      <c r="M98" s="38"/>
+      <c r="N98" s="38"/>
+      <c r="O98" s="38"/>
+      <c r="P98" s="38"/>
+      <c r="Q98" s="38"/>
+      <c r="R98" s="38"/>
+      <c r="S98" s="38"/>
+      <c r="T98" s="38"/>
+      <c r="U98" s="38"/>
+      <c r="V98" s="38"/>
+      <c r="W98" s="38"/>
+      <c r="X98" s="38"/>
+      <c r="Y98" s="38"/>
+      <c r="Z98" s="38"/>
+      <c r="AA98" s="38"/>
+      <c r="AB98" s="38"/>
+      <c r="AC98" s="38"/>
+      <c r="AD98" s="38"/>
+      <c r="AE98" s="38"/>
+      <c r="AF98" s="38"/>
+      <c r="AG98" s="38"/>
+      <c r="AH98" s="38"/>
+      <c r="AI98" s="38"/>
+      <c r="AJ98" s="38"/>
+      <c r="AK98" s="38"/>
+      <c r="AL98" s="38"/>
+      <c r="AM98" s="38"/>
+      <c r="AN98" s="38"/>
+      <c r="AO98" s="38"/>
+      <c r="AP98" s="38"/>
+      <c r="AQ98" s="38"/>
+      <c r="AR98" s="38"/>
+      <c r="AS98" s="38"/>
+      <c r="AT98" s="38"/>
+      <c r="AU98" s="38"/>
+      <c r="AV98" s="38"/>
+      <c r="AW98" s="38"/>
+      <c r="AX98" s="38"/>
+      <c r="AY98" s="38"/>
+      <c r="AZ98" s="38"/>
+      <c r="BA98" s="38"/>
+      <c r="BB98" s="38"/>
+      <c r="BC98" s="38"/>
+      <c r="BD98" s="38"/>
+      <c r="BE98" s="38"/>
+      <c r="BF98" s="38"/>
+      <c r="BG98" s="38"/>
+      <c r="BH98" s="38"/>
+      <c r="BI98" s="38"/>
+      <c r="BJ98" s="38"/>
+      <c r="BK98" s="38"/>
+      <c r="BL98" s="38"/>
+      <c r="BM98" s="38"/>
+      <c r="BN98" s="38"/>
+      <c r="BO98" s="38"/>
+      <c r="BP98" s="38"/>
+      <c r="BQ98" s="38"/>
+      <c r="BR98" s="38"/>
+      <c r="BS98" s="38"/>
+      <c r="BT98" s="38"/>
+      <c r="BU98" s="38"/>
+      <c r="BV98" s="38"/>
+      <c r="BW98" s="38"/>
+      <c r="BX98" s="38"/>
+      <c r="BY98" s="38"/>
+      <c r="BZ98" s="38"/>
+    </row>
+    <row r="99" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="72"/>
+      <c r="B99" s="59"/>
+      <c r="C99" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D98" s="61"/>
-      <c r="E98" s="62"/>
-      <c r="F98" s="62"/>
-      <c r="G98" s="63"/>
-      <c r="H98" s="64"/>
-      <c r="I98" s="65"/>
-      <c r="J98" s="66"/>
-      <c r="K98" s="67"/>
-      <c r="L98" s="67"/>
-      <c r="M98" s="67"/>
-      <c r="N98" s="68"/>
-      <c r="O98" s="68"/>
-      <c r="P98" s="68"/>
-      <c r="Q98" s="68"/>
-      <c r="R98" s="68"/>
-      <c r="S98" s="67"/>
-      <c r="T98" s="67"/>
-      <c r="U98" s="67"/>
-      <c r="V98" s="67"/>
-      <c r="W98" s="67"/>
-      <c r="X98" s="67"/>
-      <c r="Y98" s="67"/>
-      <c r="Z98" s="67"/>
-      <c r="AA98" s="67"/>
-      <c r="AB98" s="67"/>
-      <c r="AC98" s="69"/>
-      <c r="AD98" s="69"/>
-      <c r="AE98" s="69"/>
-      <c r="AF98" s="69"/>
-      <c r="AG98" s="69"/>
-      <c r="AH98" s="67"/>
-      <c r="AI98" s="67"/>
-      <c r="AJ98" s="67"/>
-      <c r="AK98" s="67"/>
-      <c r="AL98" s="67"/>
-      <c r="AM98" s="67"/>
-      <c r="AN98" s="67"/>
-      <c r="AO98" s="67"/>
-      <c r="AP98" s="67"/>
-      <c r="AQ98" s="67"/>
-      <c r="AR98" s="70"/>
-      <c r="AS98" s="70"/>
-      <c r="AT98" s="70"/>
-      <c r="AU98" s="70"/>
-      <c r="AV98" s="70"/>
-      <c r="AW98" s="67"/>
-      <c r="AX98" s="67"/>
-      <c r="AY98" s="67"/>
-      <c r="AZ98" s="67"/>
-      <c r="BA98" s="67"/>
-      <c r="BB98" s="67"/>
-      <c r="BC98" s="67"/>
-      <c r="BD98" s="67"/>
-      <c r="BE98" s="67"/>
-      <c r="BF98" s="67"/>
-      <c r="BG98" s="71"/>
-      <c r="BH98" s="71"/>
-      <c r="BI98" s="71"/>
-      <c r="BJ98" s="71"/>
-      <c r="BK98" s="71"/>
-      <c r="BL98" s="67"/>
-      <c r="BM98" s="67"/>
-      <c r="BN98" s="67"/>
-      <c r="BO98" s="67"/>
-      <c r="BP98" s="67"/>
-      <c r="BQ98" s="67"/>
-      <c r="BR98" s="67"/>
-      <c r="BS98" s="67"/>
-      <c r="BT98" s="67"/>
-      <c r="BU98" s="67"/>
-      <c r="BV98" s="67"/>
-      <c r="BW98" s="67"/>
-      <c r="BX98" s="67"/>
-      <c r="BY98" s="67"/>
-      <c r="BZ98" s="67"/>
-    </row>
-    <row r="99" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
-      <c r="B99" s="53"/>
-      <c r="C99" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="D99" s="54"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="37"/>
-      <c r="I99" s="42"/>
-      <c r="J99" s="43"/>
-      <c r="K99" s="38"/>
-      <c r="L99" s="38"/>
-      <c r="M99" s="38"/>
-      <c r="N99" s="44"/>
-      <c r="O99" s="44"/>
-      <c r="P99" s="44"/>
-      <c r="Q99" s="44"/>
-      <c r="R99" s="44"/>
-      <c r="S99" s="38"/>
-      <c r="T99" s="38"/>
-      <c r="U99" s="38"/>
-      <c r="V99" s="38"/>
-      <c r="W99" s="38"/>
-      <c r="X99" s="38"/>
-      <c r="Y99" s="38"/>
-      <c r="Z99" s="38"/>
-      <c r="AA99" s="38"/>
-      <c r="AB99" s="38"/>
-      <c r="AC99" s="39"/>
-      <c r="AD99" s="39"/>
-      <c r="AE99" s="39"/>
-      <c r="AF99" s="39"/>
-      <c r="AG99" s="39"/>
-      <c r="AH99" s="124"/>
-      <c r="AI99" s="124"/>
-      <c r="AJ99" s="124"/>
-      <c r="AK99" s="124"/>
-      <c r="AL99" s="124"/>
-      <c r="AM99" s="58"/>
-      <c r="AN99" s="38"/>
-      <c r="AO99" s="38"/>
-      <c r="AP99" s="38"/>
-      <c r="AQ99" s="38"/>
-      <c r="AR99" s="40"/>
-      <c r="AS99" s="40"/>
-      <c r="AT99" s="40"/>
-      <c r="AU99" s="40"/>
-      <c r="AV99" s="40"/>
-      <c r="AW99" s="38"/>
-      <c r="AX99" s="38"/>
-      <c r="AY99" s="38"/>
-      <c r="AZ99" s="38"/>
-      <c r="BA99" s="38"/>
-      <c r="BB99" s="38"/>
-      <c r="BC99" s="38"/>
-      <c r="BD99" s="38"/>
-      <c r="BE99" s="38"/>
-      <c r="BF99" s="38"/>
-      <c r="BG99" s="41"/>
-      <c r="BH99" s="41"/>
-      <c r="BI99" s="41"/>
-      <c r="BJ99" s="41"/>
-      <c r="BK99" s="41"/>
-      <c r="BL99" s="38"/>
-      <c r="BM99" s="38"/>
-      <c r="BN99" s="38"/>
-      <c r="BO99" s="38"/>
-      <c r="BP99" s="38"/>
-      <c r="BQ99" s="38"/>
-      <c r="BR99" s="38"/>
-      <c r="BS99" s="38"/>
-      <c r="BT99" s="38"/>
-      <c r="BU99" s="38"/>
-      <c r="BV99" s="38"/>
-      <c r="BW99" s="38"/>
-      <c r="BX99" s="38"/>
-      <c r="BY99" s="38"/>
-      <c r="BZ99" s="38"/>
+      <c r="D99" s="61"/>
+      <c r="E99" s="62"/>
+      <c r="F99" s="62"/>
+      <c r="G99" s="63"/>
+      <c r="H99" s="64"/>
+      <c r="I99" s="65"/>
+      <c r="J99" s="66"/>
+      <c r="K99" s="67"/>
+      <c r="L99" s="67"/>
+      <c r="M99" s="67"/>
+      <c r="N99" s="68"/>
+      <c r="O99" s="68"/>
+      <c r="P99" s="68"/>
+      <c r="Q99" s="68"/>
+      <c r="R99" s="68"/>
+      <c r="S99" s="67"/>
+      <c r="T99" s="67"/>
+      <c r="U99" s="67"/>
+      <c r="V99" s="67"/>
+      <c r="W99" s="67"/>
+      <c r="X99" s="67"/>
+      <c r="Y99" s="67"/>
+      <c r="Z99" s="67"/>
+      <c r="AA99" s="67"/>
+      <c r="AB99" s="67"/>
+      <c r="AC99" s="69"/>
+      <c r="AD99" s="69"/>
+      <c r="AE99" s="69"/>
+      <c r="AF99" s="69"/>
+      <c r="AG99" s="69"/>
+      <c r="AH99" s="67"/>
+      <c r="AI99" s="67"/>
+      <c r="AJ99" s="67"/>
+      <c r="AK99" s="67"/>
+      <c r="AL99" s="67"/>
+      <c r="AM99" s="67"/>
+      <c r="AN99" s="67"/>
+      <c r="AO99" s="67"/>
+      <c r="AP99" s="67"/>
+      <c r="AQ99" s="67"/>
+      <c r="AR99" s="70"/>
+      <c r="AS99" s="70"/>
+      <c r="AT99" s="70"/>
+      <c r="AU99" s="70"/>
+      <c r="AV99" s="70"/>
+      <c r="AW99" s="67"/>
+      <c r="AX99" s="67"/>
+      <c r="AY99" s="67"/>
+      <c r="AZ99" s="67"/>
+      <c r="BA99" s="67"/>
+      <c r="BB99" s="67"/>
+      <c r="BC99" s="67"/>
+      <c r="BD99" s="67"/>
+      <c r="BE99" s="67"/>
+      <c r="BF99" s="67"/>
+      <c r="BG99" s="71"/>
+      <c r="BH99" s="71"/>
+      <c r="BI99" s="71"/>
+      <c r="BJ99" s="71"/>
+      <c r="BK99" s="71"/>
+      <c r="BL99" s="67"/>
+      <c r="BM99" s="67"/>
+      <c r="BN99" s="67"/>
+      <c r="BO99" s="67"/>
+      <c r="BP99" s="67"/>
+      <c r="BQ99" s="67"/>
+      <c r="BR99" s="67"/>
+      <c r="BS99" s="67"/>
+      <c r="BT99" s="67"/>
+      <c r="BU99" s="67"/>
+      <c r="BV99" s="67"/>
+      <c r="BW99" s="67"/>
+      <c r="BX99" s="67"/>
+      <c r="BY99" s="67"/>
+      <c r="BZ99" s="67"/>
     </row>
     <row r="100" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="32"/>
       <c r="B100" s="53"/>
       <c r="C100" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D100" s="54"/>
       <c r="E100" s="35"/>
@@ -10504,7 +10500,7 @@
       <c r="A101" s="32"/>
       <c r="B101" s="53"/>
       <c r="C101" s="56" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="D101" s="54"/>
       <c r="E101" s="35"/>
@@ -10536,17 +10532,17 @@
       <c r="AE101" s="39"/>
       <c r="AF101" s="39"/>
       <c r="AG101" s="39"/>
-      <c r="AH101" s="38"/>
-      <c r="AI101" s="38"/>
-      <c r="AJ101" s="38"/>
-      <c r="AK101" s="38"/>
-      <c r="AL101" s="38"/>
-      <c r="AM101" s="38"/>
+      <c r="AH101" s="124"/>
+      <c r="AI101" s="124"/>
+      <c r="AJ101" s="124"/>
+      <c r="AK101" s="124"/>
+      <c r="AL101" s="124"/>
+      <c r="AM101" s="58"/>
       <c r="AN101" s="38"/>
-      <c r="AO101" s="149"/>
-      <c r="AP101" s="149"/>
-      <c r="AQ101" s="149"/>
-      <c r="AR101" s="147"/>
+      <c r="AO101" s="38"/>
+      <c r="AP101" s="38"/>
+      <c r="AQ101" s="38"/>
+      <c r="AR101" s="40"/>
       <c r="AS101" s="40"/>
       <c r="AT101" s="40"/>
       <c r="AU101" s="40"/>
@@ -10586,7 +10582,7 @@
       <c r="A102" s="32"/>
       <c r="B102" s="53"/>
       <c r="C102" s="56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D102" s="54"/>
       <c r="E102" s="35"/>
@@ -10628,12 +10624,12 @@
       <c r="AO102" s="149"/>
       <c r="AP102" s="149"/>
       <c r="AQ102" s="149"/>
-      <c r="AR102" s="149"/>
-      <c r="AS102" s="149"/>
-      <c r="AT102" s="149"/>
-      <c r="AU102" s="149"/>
-      <c r="AV102" s="149"/>
-      <c r="AW102" s="58"/>
+      <c r="AR102" s="147"/>
+      <c r="AS102" s="40"/>
+      <c r="AT102" s="40"/>
+      <c r="AU102" s="40"/>
+      <c r="AV102" s="40"/>
+      <c r="AW102" s="38"/>
       <c r="AX102" s="38"/>
       <c r="AY102" s="38"/>
       <c r="AZ102" s="38"/>
@@ -10668,7 +10664,7 @@
       <c r="A103" s="32"/>
       <c r="B103" s="53"/>
       <c r="C103" s="56" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D103" s="54"/>
       <c r="E103" s="35"/>
@@ -10707,15 +10703,15 @@
       <c r="AL103" s="38"/>
       <c r="AM103" s="38"/>
       <c r="AN103" s="38"/>
-      <c r="AO103" s="124"/>
-      <c r="AP103" s="124"/>
-      <c r="AQ103" s="150"/>
-      <c r="AR103" s="147"/>
-      <c r="AS103" s="40"/>
-      <c r="AT103" s="40"/>
-      <c r="AU103" s="40"/>
-      <c r="AV103" s="40"/>
-      <c r="AW103" s="38"/>
+      <c r="AO103" s="149"/>
+      <c r="AP103" s="149"/>
+      <c r="AQ103" s="149"/>
+      <c r="AR103" s="149"/>
+      <c r="AS103" s="149"/>
+      <c r="AT103" s="149"/>
+      <c r="AU103" s="149"/>
+      <c r="AV103" s="149"/>
+      <c r="AW103" s="58"/>
       <c r="AX103" s="38"/>
       <c r="AY103" s="38"/>
       <c r="AZ103" s="38"/>
@@ -10749,7 +10745,9 @@
     <row r="104" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="32"/>
       <c r="B104" s="53"/>
-      <c r="C104" s="56"/>
+      <c r="C104" s="56" t="s">
+        <v>130</v>
+      </c>
       <c r="D104" s="54"/>
       <c r="E104" s="35"/>
       <c r="F104" s="35"/>
@@ -10787,10 +10785,10 @@
       <c r="AL104" s="38"/>
       <c r="AM104" s="38"/>
       <c r="AN104" s="38"/>
-      <c r="AO104" s="38"/>
-      <c r="AP104" s="38"/>
-      <c r="AQ104" s="38"/>
-      <c r="AR104" s="40"/>
+      <c r="AO104" s="124"/>
+      <c r="AP104" s="124"/>
+      <c r="AQ104" s="150"/>
+      <c r="AR104" s="147"/>
       <c r="AS104" s="40"/>
       <c r="AT104" s="40"/>
       <c r="AU104" s="40"/>
@@ -10829,7 +10827,7 @@
     <row r="105" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="32"/>
       <c r="B105" s="53"/>
-      <c r="C105" s="57"/>
+      <c r="C105" s="56"/>
       <c r="D105" s="54"/>
       <c r="E105" s="35"/>
       <c r="F105" s="35"/>
@@ -10906,189 +10904,175 @@
       <c r="BY105" s="38"/>
       <c r="BZ105" s="38"/>
     </row>
-    <row r="106" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="26">
-        <v>4</v>
-      </c>
-      <c r="C106" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D106" s="28"/>
-      <c r="E106" s="28"/>
-      <c r="F106" s="28"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="28"/>
-      <c r="I106" s="29"/>
-      <c r="J106" s="30"/>
-      <c r="K106" s="31"/>
-      <c r="L106" s="31"/>
-      <c r="M106" s="29"/>
-      <c r="N106" s="29"/>
-      <c r="O106" s="29"/>
-      <c r="P106" s="29"/>
-      <c r="Q106" s="29"/>
-      <c r="R106" s="29"/>
-      <c r="S106" s="29"/>
-      <c r="T106" s="29"/>
-      <c r="U106" s="29"/>
-      <c r="V106" s="29"/>
-      <c r="W106" s="29"/>
-      <c r="X106" s="29"/>
-      <c r="Y106" s="29"/>
-      <c r="Z106" s="29"/>
-      <c r="AA106" s="29"/>
-      <c r="AB106" s="29"/>
-      <c r="AC106" s="29"/>
-      <c r="AD106" s="29"/>
-      <c r="AE106" s="29"/>
-      <c r="AF106" s="29"/>
-      <c r="AG106" s="29"/>
-      <c r="AH106" s="29"/>
-      <c r="AI106" s="29"/>
-      <c r="AJ106" s="29"/>
-      <c r="AK106" s="29"/>
-      <c r="AL106" s="29"/>
-      <c r="AM106" s="29"/>
-      <c r="AN106" s="29"/>
-      <c r="AO106" s="29"/>
-      <c r="AP106" s="29"/>
-      <c r="AQ106" s="29"/>
-      <c r="AR106" s="29"/>
-      <c r="AS106" s="29"/>
-      <c r="AT106" s="29"/>
-      <c r="AU106" s="29"/>
-      <c r="AV106" s="29"/>
-      <c r="AW106" s="29"/>
-      <c r="AX106" s="29"/>
-      <c r="AY106" s="29"/>
-      <c r="AZ106" s="29"/>
-      <c r="BA106" s="29"/>
-      <c r="BB106" s="29"/>
-      <c r="BC106" s="29"/>
-      <c r="BD106" s="29"/>
-      <c r="BE106" s="29"/>
-      <c r="BF106" s="29"/>
-      <c r="BG106" s="29"/>
-      <c r="BH106" s="29"/>
-      <c r="BI106" s="29"/>
-      <c r="BJ106" s="29"/>
-      <c r="BK106" s="29"/>
-      <c r="BL106" s="29"/>
-      <c r="BM106" s="29"/>
-      <c r="BN106" s="29"/>
-      <c r="BO106" s="29"/>
-      <c r="BP106" s="29"/>
-      <c r="BQ106" s="29"/>
-      <c r="BR106" s="29"/>
-      <c r="BS106" s="29"/>
-      <c r="BT106" s="29"/>
-      <c r="BU106" s="29"/>
-      <c r="BV106" s="29"/>
-      <c r="BW106" s="29"/>
-      <c r="BX106" s="29"/>
-      <c r="BY106" s="29"/>
-      <c r="BZ106" s="29"/>
+    <row r="106" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="32"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="54"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="35"/>
+      <c r="G106" s="36"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="42"/>
+      <c r="J106" s="43"/>
+      <c r="K106" s="38"/>
+      <c r="L106" s="38"/>
+      <c r="M106" s="38"/>
+      <c r="N106" s="44"/>
+      <c r="O106" s="44"/>
+      <c r="P106" s="44"/>
+      <c r="Q106" s="44"/>
+      <c r="R106" s="44"/>
+      <c r="S106" s="38"/>
+      <c r="T106" s="38"/>
+      <c r="U106" s="38"/>
+      <c r="V106" s="38"/>
+      <c r="W106" s="38"/>
+      <c r="X106" s="38"/>
+      <c r="Y106" s="38"/>
+      <c r="Z106" s="38"/>
+      <c r="AA106" s="38"/>
+      <c r="AB106" s="38"/>
+      <c r="AC106" s="39"/>
+      <c r="AD106" s="39"/>
+      <c r="AE106" s="39"/>
+      <c r="AF106" s="39"/>
+      <c r="AG106" s="39"/>
+      <c r="AH106" s="38"/>
+      <c r="AI106" s="38"/>
+      <c r="AJ106" s="38"/>
+      <c r="AK106" s="38"/>
+      <c r="AL106" s="38"/>
+      <c r="AM106" s="38"/>
+      <c r="AN106" s="38"/>
+      <c r="AO106" s="38"/>
+      <c r="AP106" s="38"/>
+      <c r="AQ106" s="38"/>
+      <c r="AR106" s="40"/>
+      <c r="AS106" s="40"/>
+      <c r="AT106" s="40"/>
+      <c r="AU106" s="40"/>
+      <c r="AV106" s="40"/>
+      <c r="AW106" s="38"/>
+      <c r="AX106" s="38"/>
+      <c r="AY106" s="38"/>
+      <c r="AZ106" s="38"/>
+      <c r="BA106" s="38"/>
+      <c r="BB106" s="38"/>
+      <c r="BC106" s="38"/>
+      <c r="BD106" s="38"/>
+      <c r="BE106" s="38"/>
+      <c r="BF106" s="38"/>
+      <c r="BG106" s="41"/>
+      <c r="BH106" s="41"/>
+      <c r="BI106" s="41"/>
+      <c r="BJ106" s="41"/>
+      <c r="BK106" s="41"/>
+      <c r="BL106" s="38"/>
+      <c r="BM106" s="38"/>
+      <c r="BN106" s="38"/>
+      <c r="BO106" s="38"/>
+      <c r="BP106" s="38"/>
+      <c r="BQ106" s="38"/>
+      <c r="BR106" s="38"/>
+      <c r="BS106" s="38"/>
+      <c r="BT106" s="38"/>
+      <c r="BU106" s="38"/>
+      <c r="BV106" s="38"/>
+      <c r="BW106" s="38"/>
+      <c r="BX106" s="38"/>
+      <c r="BY106" s="38"/>
+      <c r="BZ106" s="38"/>
     </row>
     <row r="107" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C107" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="D107" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E107" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F107" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="G107" s="36" t="e">
-        <f>DAYS360(E107,F107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H107" s="37">
-        <v>1</v>
-      </c>
-      <c r="I107" s="42"/>
-      <c r="J107" s="43"/>
-      <c r="K107" s="38"/>
-      <c r="L107" s="38"/>
-      <c r="M107" s="38"/>
-      <c r="N107" s="44"/>
-      <c r="O107" s="44"/>
-      <c r="P107" s="44"/>
-      <c r="Q107" s="44"/>
-      <c r="R107" s="44"/>
-      <c r="S107" s="38"/>
-      <c r="T107" s="38"/>
-      <c r="U107" s="38"/>
-      <c r="V107" s="38"/>
-      <c r="W107" s="38"/>
-      <c r="X107" s="38"/>
-      <c r="Y107" s="38"/>
-      <c r="Z107" s="38"/>
-      <c r="AA107" s="38"/>
-      <c r="AB107" s="38"/>
-      <c r="AC107" s="39"/>
-      <c r="AD107" s="39"/>
-      <c r="AE107" s="39"/>
-      <c r="AF107" s="39"/>
-      <c r="AG107" s="39"/>
-      <c r="AH107" s="38"/>
-      <c r="AI107" s="38"/>
-      <c r="AJ107" s="38"/>
-      <c r="AK107" s="38"/>
-      <c r="AL107" s="38"/>
-      <c r="AM107" s="38"/>
-      <c r="AN107" s="38"/>
-      <c r="AO107" s="38"/>
-      <c r="AP107" s="38"/>
-      <c r="AQ107" s="38"/>
-      <c r="AR107" s="40"/>
-      <c r="AS107" s="40"/>
-      <c r="AT107" s="40"/>
-      <c r="AU107" s="40"/>
-      <c r="AV107" s="40"/>
-      <c r="AW107" s="38"/>
-      <c r="AX107" s="38"/>
-      <c r="AY107" s="38"/>
-      <c r="AZ107" s="38"/>
-      <c r="BA107" s="38"/>
-      <c r="BB107" s="38"/>
-      <c r="BC107" s="38"/>
-      <c r="BD107" s="38"/>
-      <c r="BE107" s="38"/>
-      <c r="BF107" s="38"/>
-      <c r="BG107" s="41"/>
-      <c r="BH107" s="41"/>
-      <c r="BI107" s="41"/>
-      <c r="BJ107" s="41"/>
-      <c r="BK107" s="41"/>
-      <c r="BL107" s="38"/>
-      <c r="BM107" s="38"/>
-      <c r="BN107" s="38"/>
-      <c r="BO107" s="38"/>
-      <c r="BP107" s="38"/>
-      <c r="BQ107" s="38"/>
-      <c r="BR107" s="38"/>
-      <c r="BS107" s="38"/>
-      <c r="BT107" s="38"/>
-      <c r="BU107" s="38"/>
-      <c r="BV107" s="38"/>
-      <c r="BW107" s="38"/>
-      <c r="BX107" s="38"/>
-      <c r="BY107" s="38"/>
-      <c r="BZ107" s="38"/>
+      <c r="B107" s="26">
+        <v>4</v>
+      </c>
+      <c r="C107" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="D107" s="28"/>
+      <c r="E107" s="28"/>
+      <c r="F107" s="28"/>
+      <c r="G107" s="28"/>
+      <c r="H107" s="28"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="30"/>
+      <c r="K107" s="31"/>
+      <c r="L107" s="31"/>
+      <c r="M107" s="29"/>
+      <c r="N107" s="29"/>
+      <c r="O107" s="29"/>
+      <c r="P107" s="29"/>
+      <c r="Q107" s="29"/>
+      <c r="R107" s="29"/>
+      <c r="S107" s="29"/>
+      <c r="T107" s="29"/>
+      <c r="U107" s="29"/>
+      <c r="V107" s="29"/>
+      <c r="W107" s="29"/>
+      <c r="X107" s="29"/>
+      <c r="Y107" s="29"/>
+      <c r="Z107" s="29"/>
+      <c r="AA107" s="29"/>
+      <c r="AB107" s="29"/>
+      <c r="AC107" s="29"/>
+      <c r="AD107" s="29"/>
+      <c r="AE107" s="29"/>
+      <c r="AF107" s="29"/>
+      <c r="AG107" s="29"/>
+      <c r="AH107" s="29"/>
+      <c r="AI107" s="29"/>
+      <c r="AJ107" s="29"/>
+      <c r="AK107" s="29"/>
+      <c r="AL107" s="29"/>
+      <c r="AM107" s="29"/>
+      <c r="AN107" s="29"/>
+      <c r="AO107" s="29"/>
+      <c r="AP107" s="29"/>
+      <c r="AQ107" s="29"/>
+      <c r="AR107" s="29"/>
+      <c r="AS107" s="29"/>
+      <c r="AT107" s="29"/>
+      <c r="AU107" s="29"/>
+      <c r="AV107" s="29"/>
+      <c r="AW107" s="29"/>
+      <c r="AX107" s="29"/>
+      <c r="AY107" s="29"/>
+      <c r="AZ107" s="29"/>
+      <c r="BA107" s="29"/>
+      <c r="BB107" s="29"/>
+      <c r="BC107" s="29"/>
+      <c r="BD107" s="29"/>
+      <c r="BE107" s="29"/>
+      <c r="BF107" s="29"/>
+      <c r="BG107" s="29"/>
+      <c r="BH107" s="29"/>
+      <c r="BI107" s="29"/>
+      <c r="BJ107" s="29"/>
+      <c r="BK107" s="29"/>
+      <c r="BL107" s="29"/>
+      <c r="BM107" s="29"/>
+      <c r="BN107" s="29"/>
+      <c r="BO107" s="29"/>
+      <c r="BP107" s="29"/>
+      <c r="BQ107" s="29"/>
+      <c r="BR107" s="29"/>
+      <c r="BS107" s="29"/>
+      <c r="BT107" s="29"/>
+      <c r="BU107" s="29"/>
+      <c r="BV107" s="29"/>
+      <c r="BW107" s="29"/>
+      <c r="BX107" s="29"/>
+      <c r="BY107" s="29"/>
+      <c r="BZ107" s="29"/>
     </row>
     <row r="108" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="33">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C108" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D108" s="34" t="s">
         <v>18</v>
@@ -11099,8 +11083,9 @@
       <c r="F108" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G108" s="36">
-        <v>0</v>
+      <c r="G108" s="36" t="e">
+        <f>DAYS360(E108,F108)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H108" s="37">
         <v>1</v>
@@ -11177,23 +11162,22 @@
       <c r="BZ108" s="38"/>
     </row>
     <row r="109" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="33" t="s">
-        <v>47</v>
+      <c r="B109" s="33">
+        <v>4.2</v>
       </c>
       <c r="C109" s="47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D109" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E109" s="35">
-        <v>44823</v>
-      </c>
-      <c r="F109" s="35">
-        <v>44823</v>
+      <c r="E109" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F109" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="G109" s="36">
-        <f t="shared" ref="G109:G113" si="4">DAYS360(E109,F109)</f>
         <v>0</v>
       </c>
       <c r="H109" s="37">
@@ -11272,25 +11256,25 @@
     </row>
     <row r="110" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C110" s="47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D110" s="34" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E110" s="35">
-        <v>44829</v>
+        <v>44823</v>
       </c>
       <c r="F110" s="35">
-        <v>44829</v>
+        <v>44823</v>
       </c>
       <c r="G110" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G110:G114" si="4">DAYS360(E110,F110)</f>
         <v>0</v>
       </c>
-      <c r="H110" s="52">
+      <c r="H110" s="37">
         <v>1</v>
       </c>
       <c r="I110" s="42"/>
@@ -11366,25 +11350,25 @@
     </row>
     <row r="111" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C111" s="47" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D111" s="34" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E111" s="35">
-        <v>44830</v>
+        <v>44829</v>
       </c>
       <c r="F111" s="35">
-        <v>44830</v>
+        <v>44829</v>
       </c>
       <c r="G111" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H111" s="37">
+      <c r="H111" s="52">
         <v>1</v>
       </c>
       <c r="I111" s="42"/>
@@ -11460,19 +11444,19 @@
     </row>
     <row r="112" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="33" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C112" s="47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D112" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E112" s="35">
-        <v>44837</v>
+        <v>44830</v>
       </c>
       <c r="F112" s="35">
-        <v>44837</v>
+        <v>44830</v>
       </c>
       <c r="G112" s="36">
         <f t="shared" si="4"/>
@@ -11553,18 +11537,20 @@
       <c r="BZ112" s="38"/>
     </row>
     <row r="113" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="33"/>
+      <c r="B113" s="33" t="s">
+        <v>62</v>
+      </c>
       <c r="C113" s="47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D113" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E113" s="35">
-        <v>44844</v>
+        <v>44837</v>
       </c>
       <c r="F113" s="35">
-        <v>44844</v>
+        <v>44837</v>
       </c>
       <c r="G113" s="36">
         <f t="shared" si="4"/>
@@ -11645,11 +11631,9 @@
       <c r="BZ113" s="38"/>
     </row>
     <row r="114" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C114" s="106" t="s">
-        <v>92</v>
+      <c r="B114" s="33"/>
+      <c r="C114" s="47" t="s">
+        <v>65</v>
       </c>
       <c r="D114" s="34" t="s">
         <v>18</v>
@@ -11661,7 +11645,7 @@
         <v>44844</v>
       </c>
       <c r="G114" s="36">
-        <f t="shared" ref="G114" si="5">DAYS360(E114,F114)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H114" s="37">
@@ -11739,106 +11723,180 @@
       <c r="BZ114" s="38"/>
     </row>
     <row r="115" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="107"/>
-      <c r="C115" s="108"/>
-      <c r="D115" s="109"/>
-      <c r="E115" s="110"/>
-      <c r="F115" s="110"/>
-      <c r="G115" s="111"/>
-      <c r="H115" s="112"/>
-      <c r="I115" s="113"/>
-      <c r="J115" s="114"/>
-      <c r="K115" s="115"/>
-      <c r="L115" s="115"/>
-      <c r="M115" s="115"/>
-      <c r="N115" s="116"/>
-      <c r="O115" s="116"/>
-      <c r="P115" s="116"/>
-      <c r="Q115" s="116"/>
-      <c r="R115" s="116"/>
-      <c r="S115" s="115"/>
-      <c r="T115" s="115"/>
-      <c r="U115" s="115"/>
-      <c r="V115" s="115"/>
-      <c r="W115" s="115"/>
-      <c r="X115" s="115"/>
-      <c r="Y115" s="115"/>
-      <c r="Z115" s="115"/>
-      <c r="AA115" s="115"/>
-      <c r="AB115" s="115"/>
-      <c r="AC115" s="117"/>
-      <c r="AD115" s="117"/>
-      <c r="AE115" s="117"/>
-      <c r="AF115" s="117"/>
-      <c r="AG115" s="117"/>
-      <c r="AH115" s="115"/>
-      <c r="AI115" s="115"/>
-      <c r="AJ115" s="115"/>
-      <c r="AK115" s="115"/>
-      <c r="AL115" s="115"/>
-      <c r="AM115" s="115"/>
-      <c r="AN115" s="115"/>
-      <c r="AO115" s="115"/>
-      <c r="AP115" s="115"/>
-      <c r="AQ115" s="115"/>
-      <c r="AR115" s="118"/>
-      <c r="AS115" s="118"/>
-      <c r="AT115" s="118"/>
-      <c r="AU115" s="118"/>
-      <c r="AV115" s="118"/>
-      <c r="AW115" s="115"/>
-      <c r="AX115" s="115"/>
-      <c r="AY115" s="115"/>
-      <c r="AZ115" s="115"/>
-      <c r="BA115" s="115"/>
-      <c r="BB115" s="115"/>
-      <c r="BC115" s="115"/>
-      <c r="BD115" s="115"/>
-      <c r="BE115" s="115"/>
-      <c r="BF115" s="115"/>
-      <c r="BG115" s="119"/>
-      <c r="BH115" s="119"/>
-      <c r="BI115" s="119"/>
-      <c r="BJ115" s="119"/>
-      <c r="BK115" s="119"/>
-      <c r="BL115" s="115"/>
-      <c r="BM115" s="115"/>
-      <c r="BN115" s="115"/>
-      <c r="BO115" s="115"/>
-      <c r="BP115" s="115"/>
-      <c r="BQ115" s="115"/>
-      <c r="BR115" s="115"/>
-      <c r="BS115" s="115"/>
-      <c r="BT115" s="115"/>
-      <c r="BU115" s="115"/>
-      <c r="BV115" s="115"/>
-      <c r="BW115" s="115"/>
-      <c r="BX115" s="115"/>
-      <c r="BY115" s="115"/>
-      <c r="BZ115" s="115"/>
+      <c r="B115" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C115" s="106" t="s">
+        <v>92</v>
+      </c>
+      <c r="D115" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="35">
+        <v>44844</v>
+      </c>
+      <c r="F115" s="35">
+        <v>44844</v>
+      </c>
+      <c r="G115" s="36">
+        <f t="shared" ref="G115" si="5">DAYS360(E115,F115)</f>
+        <v>0</v>
+      </c>
+      <c r="H115" s="37">
+        <v>1</v>
+      </c>
+      <c r="I115" s="42"/>
+      <c r="J115" s="43"/>
+      <c r="K115" s="38"/>
+      <c r="L115" s="38"/>
+      <c r="M115" s="38"/>
+      <c r="N115" s="44"/>
+      <c r="O115" s="44"/>
+      <c r="P115" s="44"/>
+      <c r="Q115" s="44"/>
+      <c r="R115" s="44"/>
+      <c r="S115" s="38"/>
+      <c r="T115" s="38"/>
+      <c r="U115" s="38"/>
+      <c r="V115" s="38"/>
+      <c r="W115" s="38"/>
+      <c r="X115" s="38"/>
+      <c r="Y115" s="38"/>
+      <c r="Z115" s="38"/>
+      <c r="AA115" s="38"/>
+      <c r="AB115" s="38"/>
+      <c r="AC115" s="39"/>
+      <c r="AD115" s="39"/>
+      <c r="AE115" s="39"/>
+      <c r="AF115" s="39"/>
+      <c r="AG115" s="39"/>
+      <c r="AH115" s="38"/>
+      <c r="AI115" s="38"/>
+      <c r="AJ115" s="38"/>
+      <c r="AK115" s="38"/>
+      <c r="AL115" s="38"/>
+      <c r="AM115" s="38"/>
+      <c r="AN115" s="38"/>
+      <c r="AO115" s="38"/>
+      <c r="AP115" s="38"/>
+      <c r="AQ115" s="38"/>
+      <c r="AR115" s="40"/>
+      <c r="AS115" s="40"/>
+      <c r="AT115" s="40"/>
+      <c r="AU115" s="40"/>
+      <c r="AV115" s="40"/>
+      <c r="AW115" s="38"/>
+      <c r="AX115" s="38"/>
+      <c r="AY115" s="38"/>
+      <c r="AZ115" s="38"/>
+      <c r="BA115" s="38"/>
+      <c r="BB115" s="38"/>
+      <c r="BC115" s="38"/>
+      <c r="BD115" s="38"/>
+      <c r="BE115" s="38"/>
+      <c r="BF115" s="38"/>
+      <c r="BG115" s="41"/>
+      <c r="BH115" s="41"/>
+      <c r="BI115" s="41"/>
+      <c r="BJ115" s="41"/>
+      <c r="BK115" s="41"/>
+      <c r="BL115" s="38"/>
+      <c r="BM115" s="38"/>
+      <c r="BN115" s="38"/>
+      <c r="BO115" s="38"/>
+      <c r="BP115" s="38"/>
+      <c r="BQ115" s="38"/>
+      <c r="BR115" s="38"/>
+      <c r="BS115" s="38"/>
+      <c r="BT115" s="38"/>
+      <c r="BU115" s="38"/>
+      <c r="BV115" s="38"/>
+      <c r="BW115" s="38"/>
+      <c r="BX115" s="38"/>
+      <c r="BY115" s="38"/>
+      <c r="BZ115" s="38"/>
+    </row>
+    <row r="116" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="107"/>
+      <c r="C116" s="108"/>
+      <c r="D116" s="109"/>
+      <c r="E116" s="110"/>
+      <c r="F116" s="110"/>
+      <c r="G116" s="111"/>
+      <c r="H116" s="112"/>
+      <c r="I116" s="113"/>
+      <c r="J116" s="114"/>
+      <c r="K116" s="115"/>
+      <c r="L116" s="115"/>
+      <c r="M116" s="115"/>
+      <c r="N116" s="116"/>
+      <c r="O116" s="116"/>
+      <c r="P116" s="116"/>
+      <c r="Q116" s="116"/>
+      <c r="R116" s="116"/>
+      <c r="S116" s="115"/>
+      <c r="T116" s="115"/>
+      <c r="U116" s="115"/>
+      <c r="V116" s="115"/>
+      <c r="W116" s="115"/>
+      <c r="X116" s="115"/>
+      <c r="Y116" s="115"/>
+      <c r="Z116" s="115"/>
+      <c r="AA116" s="115"/>
+      <c r="AB116" s="115"/>
+      <c r="AC116" s="117"/>
+      <c r="AD116" s="117"/>
+      <c r="AE116" s="117"/>
+      <c r="AF116" s="117"/>
+      <c r="AG116" s="117"/>
+      <c r="AH116" s="115"/>
+      <c r="AI116" s="115"/>
+      <c r="AJ116" s="115"/>
+      <c r="AK116" s="115"/>
+      <c r="AL116" s="115"/>
+      <c r="AM116" s="115"/>
+      <c r="AN116" s="115"/>
+      <c r="AO116" s="115"/>
+      <c r="AP116" s="115"/>
+      <c r="AQ116" s="115"/>
+      <c r="AR116" s="118"/>
+      <c r="AS116" s="118"/>
+      <c r="AT116" s="118"/>
+      <c r="AU116" s="118"/>
+      <c r="AV116" s="118"/>
+      <c r="AW116" s="115"/>
+      <c r="AX116" s="115"/>
+      <c r="AY116" s="115"/>
+      <c r="AZ116" s="115"/>
+      <c r="BA116" s="115"/>
+      <c r="BB116" s="115"/>
+      <c r="BC116" s="115"/>
+      <c r="BD116" s="115"/>
+      <c r="BE116" s="115"/>
+      <c r="BF116" s="115"/>
+      <c r="BG116" s="119"/>
+      <c r="BH116" s="119"/>
+      <c r="BI116" s="119"/>
+      <c r="BJ116" s="119"/>
+      <c r="BK116" s="119"/>
+      <c r="BL116" s="115"/>
+      <c r="BM116" s="115"/>
+      <c r="BN116" s="115"/>
+      <c r="BO116" s="115"/>
+      <c r="BP116" s="115"/>
+      <c r="BQ116" s="115"/>
+      <c r="BR116" s="115"/>
+      <c r="BS116" s="115"/>
+      <c r="BT116" s="115"/>
+      <c r="BU116" s="115"/>
+      <c r="BV116" s="115"/>
+      <c r="BW116" s="115"/>
+      <c r="BX116" s="115"/>
+      <c r="BY116" s="115"/>
+      <c r="BZ116" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:W9"/>
-    <mergeCell ref="X9:AL9"/>
-    <mergeCell ref="AM9:BA9"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="AC10:AG10"/>
-    <mergeCell ref="AH10:AL10"/>
-    <mergeCell ref="AM10:AQ10"/>
-    <mergeCell ref="AR10:AV10"/>
-    <mergeCell ref="AW10:BA10"/>
     <mergeCell ref="BB9:BZ9"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="N10:R10"/>
@@ -11855,10 +11913,30 @@
     <mergeCell ref="BQ10:BU10"/>
     <mergeCell ref="BV10:BZ10"/>
     <mergeCell ref="S10:W10"/>
+    <mergeCell ref="AM9:BA9"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="AC10:AG10"/>
+    <mergeCell ref="AH10:AL10"/>
+    <mergeCell ref="AM10:AQ10"/>
+    <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="AW10:BA10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:W9"/>
+    <mergeCell ref="X9:AL9"/>
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
-  <conditionalFormatting sqref="H12:H21 H23:H115">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="H12:H21 H23:H116">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11867,8 +11945,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H21 H23:H115">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="H12:H21 H23:H116">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11883,6 +11961,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7EF2104F2CEFE4DACFBF5BA7D93FB4D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb0ed258f694207805e211ca255f9b46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b71f768-6d8b-468c-a986-1e1afc74f0e3" xmlns:ns4="d07d918a-d172-4450-8f4a-7b087689ff85" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c03c9fe975be0719773112499dde791" ns3:_="" ns4:_="">
     <xsd:import namespace="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
@@ -12111,36 +12204,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FABC364-430D-422C-AD85-145699D2125C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12163,9 +12230,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FABC364-430D-422C-AD85-145699D2125C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>